<commit_message>
added cities to NIR divisions
</commit_message>
<xml_diff>
--- a/FINAL-PROGRAMS/FINAL- ALS-CLC 2024 as of May 2025.xlsx
+++ b/FINAL-PROGRAMS/FINAL- ALS-CLC 2024 as of May 2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work - Lawrence\Documents\DepEd_scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work - Lawrence\Documents\DepEd_scripts\FINAL-PROGRAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F1D1E4-CCEC-457F-B307-969F3D2D8B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C121289C-F2E4-4F5D-820B-18041376E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,16 +44,16 @@
     <definedName name="\c">#N/A</definedName>
     <definedName name="___all2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="___all2" hidden="1">#REF!</definedName>
-    <definedName name="___EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="___EDU2">[1]EDU4!$G$10</definedName>
-    <definedName name="__EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="__EDU2">[1]EDU4!$G$10</definedName>
+    <definedName name="___EDU2" localSheetId="0">[1]EDU4!$G$10</definedName>
+    <definedName name="___EDU2">[2]EDU4!$G$10</definedName>
+    <definedName name="__EDU2" localSheetId="0">[1]EDU4!$G$10</definedName>
+    <definedName name="__EDU2">[2]EDU4!$G$10</definedName>
     <definedName name="_all2" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_all2" hidden="1">#REF!</definedName>
     <definedName name="_car2" localSheetId="0">#REF!</definedName>
     <definedName name="_car2">#REF!</definedName>
-    <definedName name="_EDU2" localSheetId="0">[11]EDU4!$G$10</definedName>
-    <definedName name="_EDU2">[1]EDU4!$G$10</definedName>
+    <definedName name="_EDU2" localSheetId="0">[1]EDU4!$G$10</definedName>
+    <definedName name="_EDU2">[2]EDU4!$G$10</definedName>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$1:$W$5</definedName>
@@ -98,12 +98,12 @@
     <definedName name="awrwqqe" hidden="1">#REF!</definedName>
     <definedName name="b" localSheetId="0">#REF!</definedName>
     <definedName name="b">#REF!</definedName>
-    <definedName name="CLS">[2]Baseline!$1:$1048576</definedName>
-    <definedName name="Cost" localSheetId="0">'[12]Costs and Types'!$A$1:$A$44</definedName>
-    <definedName name="Cost">'[3]Costs and Types'!$A$1:$A$44</definedName>
+    <definedName name="CLS">[3]Baseline!$1:$1048576</definedName>
+    <definedName name="Cost" localSheetId="0">'[4]Costs and Types'!$A$1:$A$44</definedName>
+    <definedName name="Cost">'[5]Costs and Types'!$A$1:$A$44</definedName>
     <definedName name="cv">#REF!</definedName>
-    <definedName name="_xlnm.Database" localSheetId="0">[13]Database!$1:$1048576</definedName>
-    <definedName name="_xlnm.Database">[4]Database!$1:$1048576</definedName>
+    <definedName name="_xlnm.Database" localSheetId="0">[6]Database!$1:$1048576</definedName>
+    <definedName name="_xlnm.Database">[7]Database!$1:$1048576</definedName>
     <definedName name="dede" localSheetId="0">#REF!</definedName>
     <definedName name="dede">#REF!</definedName>
     <definedName name="defggr" localSheetId="0">#REF!</definedName>
@@ -128,8 +128,8 @@
     <definedName name="Eight">#REF!</definedName>
     <definedName name="elem" localSheetId="0">#REF!</definedName>
     <definedName name="elem">#REF!</definedName>
-    <definedName name="enrollment_estimates" localSheetId="0">'[5]Alloc working w formula'!#REF!</definedName>
-    <definedName name="enrollment_estimates">'[5]Alloc working w formula'!#REF!</definedName>
+    <definedName name="enrollment_estimates" localSheetId="0">'[8]Alloc working w formula'!#REF!</definedName>
+    <definedName name="enrollment_estimates">'[8]Alloc working w formula'!#REF!</definedName>
     <definedName name="Enrolment" localSheetId="0">#REF!</definedName>
     <definedName name="Enrolment">#REF!</definedName>
     <definedName name="Excel_BuiltIn_Print_Area_1" localSheetId="0">#REF!</definedName>
@@ -142,8 +142,8 @@
     <definedName name="Excel_BuiltIn_Print_Titles_1">#REF!</definedName>
     <definedName name="exp" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="exp" hidden="1">#REF!</definedName>
-    <definedName name="EXPEND" localSheetId="0">[14]EDU4!$G$10</definedName>
-    <definedName name="EXPEND">[6]EDU4!$G$10</definedName>
+    <definedName name="EXPEND" localSheetId="0">[9]EDU4!$G$10</definedName>
+    <definedName name="EXPEND">[10]EDU4!$G$10</definedName>
     <definedName name="Expenditure" localSheetId="0">#REF!</definedName>
     <definedName name="Expenditure">#REF!</definedName>
     <definedName name="Expenditure_new" localSheetId="0">#REF!</definedName>
@@ -158,10 +158,10 @@
     <definedName name="Five">#REF!</definedName>
     <definedName name="four" localSheetId="0">#REF!</definedName>
     <definedName name="four">#REF!</definedName>
-    <definedName name="gfo" localSheetId="0">[15]Database!$A$3:$E$541</definedName>
-    <definedName name="gfo">[7]Database!$A$3:$E$541</definedName>
-    <definedName name="GLEN" localSheetId="0">[16]Database!$A$3:$E$541</definedName>
-    <definedName name="GLEN">[8]Database!$A$3:$E$541</definedName>
+    <definedName name="gfo" localSheetId="0">[11]Database!$A$3:$E$541</definedName>
+    <definedName name="gfo">[12]Database!$A$3:$E$541</definedName>
+    <definedName name="GLEN" localSheetId="0">[13]Database!$A$3:$E$541</definedName>
+    <definedName name="GLEN">[14]Database!$A$3:$E$541</definedName>
     <definedName name="gttt" localSheetId="0">#REF!</definedName>
     <definedName name="gttt">#REF!</definedName>
     <definedName name="HHHH" localSheetId="0">#REF!</definedName>
@@ -276,8 +276,8 @@
     <definedName name="print_area_Mil" localSheetId="0">#REF!</definedName>
     <definedName name="print_area_Mil">#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$1:$1</definedName>
-    <definedName name="Print_Titles_MI" localSheetId="0">'[17]Enrolees&amp;Graduated'!$A$1:$IV$6,'[17]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
-    <definedName name="Print_Titles_MI">'[9]Enrolees&amp;Graduated'!$A$1:$IV$6,'[9]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
+    <definedName name="Print_Titles_MI" localSheetId="0">'[15]Enrolees&amp;Graduated'!$A$1:$IV$6,'[15]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
+    <definedName name="Print_Titles_MI">'[16]Enrolees&amp;Graduated'!$A$1:$IV$6,'[16]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
     <definedName name="procured" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="procured" hidden="1">#REF!</definedName>
     <definedName name="Procurement" localSheetId="0">#REF!</definedName>
@@ -304,8 +304,8 @@
     <definedName name="rrr">#REF!</definedName>
     <definedName name="RSBP" localSheetId="0">#REF!</definedName>
     <definedName name="RSBP">#REF!</definedName>
-    <definedName name="safe" localSheetId="0">[10]SchInfo!#REF!</definedName>
-    <definedName name="safe">[10]SchInfo!#REF!</definedName>
+    <definedName name="safe" localSheetId="0">[17]SchInfo!#REF!</definedName>
+    <definedName name="safe">[17]SchInfo!#REF!</definedName>
     <definedName name="sayot" localSheetId="0">#REF!</definedName>
     <definedName name="sayot">#REF!</definedName>
     <definedName name="seco" localSheetId="0">#REF!</definedName>
@@ -936,102 +936,6 @@
       <sheetName val="Edu-5"/>
       <sheetName val="LYDS4 (2)"/>
       <sheetName val="Database"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="SchInfo"/>
-      <sheetName val="Table1"/>
-      <sheetName val="Tables2-3"/>
-      <sheetName val="Tables4-5"/>
-      <sheetName val="Table6"/>
-      <sheetName val="Table7"/>
-      <sheetName val="Table8"/>
-      <sheetName val="Tables9-10"/>
-      <sheetName val="Table11"/>
-      <sheetName val="Table12"/>
-      <sheetName val="Table13-Box1"/>
-      <sheetName val="Tables15"/>
-      <sheetName val="Box2-Table16"/>
-      <sheetName val="Box3"/>
-      <sheetName val="Tables17-18"/>
-      <sheetName val="Box4-5"/>
-      <sheetName val="Tables19-20"/>
-      <sheetName val="Box6-Table21"/>
-      <sheetName val="Table22-Box8"/>
-      <sheetName val="Boxes9-11"/>
-      <sheetName val="Table23-Box12"/>
-      <sheetName val="Boxes13-14"/>
-      <sheetName val="Alloc working w formula"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Enrolees&amp;Graduated"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="EDU4"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="EDU4"/>
-      <sheetName val="edu May -ot"/>
-      <sheetName val="LYDS4"/>
-      <sheetName val="MIMAY4"/>
-      <sheetName val="HELEN4"/>
-      <sheetName val="OT-PAYROLL"/>
-      <sheetName val="ALOBS"/>
-      <sheetName val="Edu-5"/>
-      <sheetName val="LYDS4 (2)"/>
-      <sheetName val="Database"/>
       <sheetName val="Sheet2"/>
       <sheetName val="#REF"/>
     </sheetNames>
@@ -1053,1605 +957,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="PRIORITY 2"/>
-      <sheetName val="PRIORITY 3"/>
-      <sheetName val="Costs and Types"/>
-      <sheetName val="Database"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Liminangcong"/>
-      <sheetName val="Recommendation"/>
-      <sheetName val="Liminangcong-SWA"/>
-      <sheetName val="Liminangcong-WPR"/>
-      <sheetName val="Database"/>
-      <sheetName val="Template"/>
-      <sheetName val="Summary"/>
-      <sheetName val="DataInput"/>
-      <sheetName val="1cl 7x9 modified wo ceiling "/>
-      <sheetName val="pow (final)"/>
-      <sheetName val="2cl 7x9 modified"/>
-      <sheetName val="1cl 7x9 Ramon"/>
-      <sheetName val="1cl 7x7 modified"/>
-      <sheetName val="2cl 7x7 modified"/>
-      <sheetName val="dbase"/>
-      <sheetName val="industrial"/>
-      <sheetName val="1cl 7x9 modified"/>
-      <sheetName val="3cl 7x9 modified"/>
-      <sheetName val="1cl"/>
-      <sheetName val="2cl"/>
-      <sheetName val="3cl"/>
-      <sheetName val="5cl"/>
-      <sheetName val="2sty4cl "/>
-      <sheetName val="2sty6cl "/>
-      <sheetName val="2sty8cl "/>
-      <sheetName val="3sty9cl"/>
-      <sheetName val="h.e."/>
-      <sheetName val="cr attached"/>
-      <sheetName val="cr detached"/>
-      <sheetName val="rc septic vault"/>
-      <sheetName val="chb septic vault"/>
-      <sheetName val="1cl (2)"/>
-      <sheetName val="PROGRAM of WORK"/>
-      <sheetName val="1cl 7x7 M"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_5"/>
-      <sheetName val="pow_(final)5"/>
-      <sheetName val="2cl_7x9_modified5"/>
-      <sheetName val="1cl_7x9_Ramon5"/>
-      <sheetName val="1cl_7x7_modified5"/>
-      <sheetName val="2cl_7x7_modified5"/>
-      <sheetName val="1cl_7x9_modified5"/>
-      <sheetName val="3cl_7x9_modified5"/>
-      <sheetName val="2sty4cl_5"/>
-      <sheetName val="2sty6cl_5"/>
-      <sheetName val="2sty8cl_5"/>
-      <sheetName val="h_e_5"/>
-      <sheetName val="cr_attached5"/>
-      <sheetName val="cr_detached5"/>
-      <sheetName val="rc_septic_vault5"/>
-      <sheetName val="chb_septic_vault5"/>
-      <sheetName val="1cl_(2)5"/>
-      <sheetName val="PROGRAM_of_WORK5"/>
-      <sheetName val="1cl_7x7_M5"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_"/>
-      <sheetName val="pow_(final)"/>
-      <sheetName val="2cl_7x9_modified"/>
-      <sheetName val="1cl_7x9_Ramon"/>
-      <sheetName val="1cl_7x7_modified"/>
-      <sheetName val="2cl_7x7_modified"/>
-      <sheetName val="1cl_7x9_modified"/>
-      <sheetName val="3cl_7x9_modified"/>
-      <sheetName val="2sty4cl_"/>
-      <sheetName val="2sty6cl_"/>
-      <sheetName val="2sty8cl_"/>
-      <sheetName val="h_e_"/>
-      <sheetName val="cr_attached"/>
-      <sheetName val="cr_detached"/>
-      <sheetName val="rc_septic_vault"/>
-      <sheetName val="chb_septic_vault"/>
-      <sheetName val="1cl_(2)"/>
-      <sheetName val="PROGRAM_of_WORK"/>
-      <sheetName val="1cl_7x7_M"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_1"/>
-      <sheetName val="pow_(final)1"/>
-      <sheetName val="2cl_7x9_modified1"/>
-      <sheetName val="1cl_7x9_Ramon1"/>
-      <sheetName val="1cl_7x7_modified1"/>
-      <sheetName val="2cl_7x7_modified1"/>
-      <sheetName val="1cl_7x9_modified1"/>
-      <sheetName val="3cl_7x9_modified1"/>
-      <sheetName val="2sty4cl_1"/>
-      <sheetName val="2sty6cl_1"/>
-      <sheetName val="2sty8cl_1"/>
-      <sheetName val="h_e_1"/>
-      <sheetName val="cr_attached1"/>
-      <sheetName val="cr_detached1"/>
-      <sheetName val="rc_septic_vault1"/>
-      <sheetName val="chb_septic_vault1"/>
-      <sheetName val="1cl_(2)1"/>
-      <sheetName val="PROGRAM_of_WORK1"/>
-      <sheetName val="1cl_7x7_M1"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_3"/>
-      <sheetName val="pow_(final)3"/>
-      <sheetName val="2cl_7x9_modified3"/>
-      <sheetName val="1cl_7x9_Ramon3"/>
-      <sheetName val="1cl_7x7_modified3"/>
-      <sheetName val="2cl_7x7_modified3"/>
-      <sheetName val="1cl_7x9_modified3"/>
-      <sheetName val="3cl_7x9_modified3"/>
-      <sheetName val="2sty4cl_3"/>
-      <sheetName val="2sty6cl_3"/>
-      <sheetName val="2sty8cl_3"/>
-      <sheetName val="h_e_3"/>
-      <sheetName val="cr_attached3"/>
-      <sheetName val="cr_detached3"/>
-      <sheetName val="rc_septic_vault3"/>
-      <sheetName val="chb_septic_vault3"/>
-      <sheetName val="1cl_(2)3"/>
-      <sheetName val="PROGRAM_of_WORK3"/>
-      <sheetName val="1cl_7x7_M3"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_2"/>
-      <sheetName val="pow_(final)2"/>
-      <sheetName val="2cl_7x9_modified2"/>
-      <sheetName val="1cl_7x9_Ramon2"/>
-      <sheetName val="1cl_7x7_modified2"/>
-      <sheetName val="2cl_7x7_modified2"/>
-      <sheetName val="1cl_7x9_modified2"/>
-      <sheetName val="3cl_7x9_modified2"/>
-      <sheetName val="2sty4cl_2"/>
-      <sheetName val="2sty6cl_2"/>
-      <sheetName val="2sty8cl_2"/>
-      <sheetName val="h_e_2"/>
-      <sheetName val="cr_attached2"/>
-      <sheetName val="cr_detached2"/>
-      <sheetName val="rc_septic_vault2"/>
-      <sheetName val="chb_septic_vault2"/>
-      <sheetName val="1cl_(2)2"/>
-      <sheetName val="PROGRAM_of_WORK2"/>
-      <sheetName val="1cl_7x7_M2"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_4"/>
-      <sheetName val="pow_(final)4"/>
-      <sheetName val="2cl_7x9_modified4"/>
-      <sheetName val="1cl_7x9_Ramon4"/>
-      <sheetName val="1cl_7x7_modified4"/>
-      <sheetName val="2cl_7x7_modified4"/>
-      <sheetName val="1cl_7x9_modified4"/>
-      <sheetName val="3cl_7x9_modified4"/>
-      <sheetName val="2sty4cl_4"/>
-      <sheetName val="2sty6cl_4"/>
-      <sheetName val="2sty8cl_4"/>
-      <sheetName val="h_e_4"/>
-      <sheetName val="cr_attached4"/>
-      <sheetName val="cr_detached4"/>
-      <sheetName val="rc_septic_vault4"/>
-      <sheetName val="chb_septic_vault4"/>
-      <sheetName val="1cl_(2)4"/>
-      <sheetName val="PROGRAM_of_WORK4"/>
-      <sheetName val="1cl_7x7_M4"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_6"/>
-      <sheetName val="pow_(final)6"/>
-      <sheetName val="2cl_7x9_modified6"/>
-      <sheetName val="1cl_7x9_Ramon6"/>
-      <sheetName val="1cl_7x7_modified6"/>
-      <sheetName val="2cl_7x7_modified6"/>
-      <sheetName val="1cl_7x9_modified6"/>
-      <sheetName val="3cl_7x9_modified6"/>
-      <sheetName val="2sty4cl_6"/>
-      <sheetName val="2sty6cl_6"/>
-      <sheetName val="2sty8cl_6"/>
-      <sheetName val="h_e_6"/>
-      <sheetName val="cr_attached6"/>
-      <sheetName val="cr_detached6"/>
-      <sheetName val="rc_septic_vault6"/>
-      <sheetName val="chb_septic_vault6"/>
-      <sheetName val="1cl_(2)6"/>
-      <sheetName val="PROGRAM_of_WORK6"/>
-      <sheetName val="1cl_7x7_M6"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_7"/>
-      <sheetName val="pow_(final)7"/>
-      <sheetName val="2cl_7x9_modified7"/>
-      <sheetName val="1cl_7x9_Ramon7"/>
-      <sheetName val="1cl_7x7_modified7"/>
-      <sheetName val="2cl_7x7_modified7"/>
-      <sheetName val="1cl_7x9_modified7"/>
-      <sheetName val="3cl_7x9_modified7"/>
-      <sheetName val="2sty4cl_7"/>
-      <sheetName val="2sty6cl_7"/>
-      <sheetName val="2sty8cl_7"/>
-      <sheetName val="h_e_7"/>
-      <sheetName val="cr_attached7"/>
-      <sheetName val="cr_detached7"/>
-      <sheetName val="rc_septic_vault7"/>
-      <sheetName val="chb_septic_vault7"/>
-      <sheetName val="1cl_(2)7"/>
-      <sheetName val="PROGRAM_of_WORK7"/>
-      <sheetName val="1cl_7x7_M7"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_8"/>
-      <sheetName val="pow_(final)8"/>
-      <sheetName val="2cl_7x9_modified8"/>
-      <sheetName val="1cl_7x9_Ramon8"/>
-      <sheetName val="1cl_7x7_modified8"/>
-      <sheetName val="2cl_7x7_modified8"/>
-      <sheetName val="1cl_7x9_modified8"/>
-      <sheetName val="3cl_7x9_modified8"/>
-      <sheetName val="2sty4cl_8"/>
-      <sheetName val="2sty6cl_8"/>
-      <sheetName val="2sty8cl_8"/>
-      <sheetName val="h_e_8"/>
-      <sheetName val="cr_attached8"/>
-      <sheetName val="cr_detached8"/>
-      <sheetName val="rc_septic_vault8"/>
-      <sheetName val="chb_septic_vault8"/>
-      <sheetName val="1cl_(2)8"/>
-      <sheetName val="PROGRAM_of_WORK8"/>
-      <sheetName val="1cl_7x7_M8"/>
-      <sheetName val="POW"/>
-      <sheetName val="repair det est"/>
-      <sheetName val="program of works"/>
-      <sheetName val="2cl 7x7 M"/>
-      <sheetName val="3cl 7x7 M"/>
-      <sheetName val="1cl 7x9 M"/>
-      <sheetName val="2cl 7x9 M"/>
-      <sheetName val="3cl 7x9 M"/>
-      <sheetName val="4cl 7x9 M"/>
-      <sheetName val="1cl 7x9 O"/>
-      <sheetName val="2cl 7x9 O"/>
-      <sheetName val="2cl 7x9 O_sphere"/>
-      <sheetName val="3cl 7x9 O"/>
-      <sheetName val="multipurpose"/>
-      <sheetName val="science lab"/>
-      <sheetName val="Typhoon Resistance_2CL"/>
-      <sheetName val="RC_SV"/>
-      <sheetName val="CHB_SV"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_9"/>
-      <sheetName val="pow_(final)9"/>
-      <sheetName val="2cl_7x9_modified9"/>
-      <sheetName val="1cl_7x9_Ramon9"/>
-      <sheetName val="1cl_7x7_modified9"/>
-      <sheetName val="2cl_7x7_modified9"/>
-      <sheetName val="1cl_7x9_modified9"/>
-      <sheetName val="3cl_7x9_modified9"/>
-      <sheetName val="2sty4cl_9"/>
-      <sheetName val="2sty6cl_9"/>
-      <sheetName val="2sty8cl_9"/>
-      <sheetName val="h_e_9"/>
-      <sheetName val="cr_attached9"/>
-      <sheetName val="cr_detached9"/>
-      <sheetName val="rc_septic_vault9"/>
-      <sheetName val="chb_septic_vault9"/>
-      <sheetName val="1cl_(2)9"/>
-      <sheetName val="PROGRAM_of_WORK9"/>
-      <sheetName val="1cl_7x7_M9"/>
-      <sheetName val="repair_det_est"/>
-      <sheetName val="program_of_works"/>
-      <sheetName val="2cl_7x7_M"/>
-      <sheetName val="3cl_7x7_M"/>
-      <sheetName val="1cl_7x9_M"/>
-      <sheetName val="2cl_7x9_M"/>
-      <sheetName val="3cl_7x9_M"/>
-      <sheetName val="4cl_7x9_M"/>
-      <sheetName val="1cl_7x9_O"/>
-      <sheetName val="2cl_7x9_O"/>
-      <sheetName val="2cl_7x9_O_sphere"/>
-      <sheetName val="3cl_7x9_O"/>
-      <sheetName val="science_lab"/>
-      <sheetName val="Typhoon_Resistance_2CL"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_10"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_11"/>
-      <sheetName val="3sty15cl-1"/>
-      <sheetName val="buhelebongES"/>
-      <sheetName val="DECS 2cl OMS (2)"/>
-      <sheetName val="COP2 okiot tabuac bcps(100)"/>
-      <sheetName val="Detailed Estimate"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="unit weight of angle bars"/>
-      <sheetName val="unit weight of purlins"/>
-      <sheetName val="NEWCON 2017 (CL)"/>
-      <sheetName val="BEFF 2016"/>
-      <sheetName val="Account Type"/>
-      <sheetName val="Source of data"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_12"/>
-      <sheetName val="pow_(final)10"/>
-      <sheetName val="2cl_7x9_modified10"/>
-      <sheetName val="1cl_7x9_Ramon10"/>
-      <sheetName val="1cl_7x7_modified10"/>
-      <sheetName val="2cl_7x7_modified10"/>
-      <sheetName val="1cl_7x9_modified10"/>
-      <sheetName val="3cl_7x9_modified10"/>
-      <sheetName val="2sty4cl_10"/>
-      <sheetName val="2sty6cl_10"/>
-      <sheetName val="2sty8cl_10"/>
-      <sheetName val="h_e_10"/>
-      <sheetName val="cr_attached10"/>
-      <sheetName val="cr_detached10"/>
-      <sheetName val="rc_septic_vault10"/>
-      <sheetName val="chb_septic_vault10"/>
-      <sheetName val="1cl_(2)10"/>
-      <sheetName val="PROGRAM_of_WORK10"/>
-      <sheetName val="1cl_7x7_M10"/>
-      <sheetName val="repair_det_est1"/>
-      <sheetName val="program_of_works1"/>
-      <sheetName val="2cl_7x7_M1"/>
-      <sheetName val="3cl_7x7_M1"/>
-      <sheetName val="1cl_7x9_M1"/>
-      <sheetName val="2cl_7x9_M1"/>
-      <sheetName val="3cl_7x9_M1"/>
-      <sheetName val="4cl_7x9_M1"/>
-      <sheetName val="1cl_7x9_O1"/>
-      <sheetName val="2cl_7x9_O1"/>
-      <sheetName val="2cl_7x9_O_sphere1"/>
-      <sheetName val="3cl_7x9_O1"/>
-      <sheetName val="science_lab1"/>
-      <sheetName val="Typhoon_Resistance_2CL1"/>
-      <sheetName val="DECS_2cl_OMS_(2)"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)"/>
-      <sheetName val="Detailed_Estimate"/>
-      <sheetName val="unit_weight_of_angle_bars"/>
-      <sheetName val="unit_weight_of_purlins"/>
-      <sheetName val="NEWCON_2017_(CL)"/>
-      <sheetName val="BEFF_2016"/>
-      <sheetName val="Account_Type"/>
-      <sheetName val="900b"/>
-      <sheetName val="900a"/>
-      <sheetName val="1cl_7x9_Ramn1"/>
-      <sheetName val="⊹≣駤_≚7≎≭믧ì⋡뭦ꫭ⋬餱"/>
-      <sheetName val="⋜ú曆衟Ùꩋᄷ}衭 d駒ÿ꫏ì蠱"/>
-      <sheetName val="1_x0005_"/>
-      <sheetName val="_Recovered_SheetName_79_"/>
-      <sheetName val="_Recovered_SheetName_80_"/>
-      <sheetName val="_Recovered_SheetName_81_"/>
-      <sheetName val="_Recovered_SheetName_82_"/>
-      <sheetName val="_Recovered_SheetName_83_"/>
-      <sheetName val="_Recovered_SheetName_84_"/>
-      <sheetName val="_Recovered_SheetName_85_"/>
-      <sheetName val="_Recovered_SheetName_86_"/>
-      <sheetName val="_Recovered_SheetName_87_"/>
-      <sheetName val="_Recovered_SheetName_88_"/>
-      <sheetName val="_Recovered_SheetName_89_"/>
-      <sheetName val="_Recovered_SheetName_90_"/>
-      <sheetName val="_Recovered_SheetName_91_"/>
-      <sheetName val="_Recovered_SheetName_92_"/>
-      <sheetName val="_Recovered_SheetName_93_"/>
-      <sheetName val="_Recovered_SheetName_94_"/>
-      <sheetName val="_Recovered_SheetName_95_"/>
-      <sheetName val="_Recovered_SheetName_96_"/>
-      <sheetName val="_Recovered_SheetName_97_"/>
-      <sheetName val="_Recovered_SheetName_98_"/>
-      <sheetName val="_Recovered_SheetName_99_"/>
-      <sheetName val="_Recovered_SheetName_100_"/>
-      <sheetName val="_Recovered_SheetName_101_"/>
-      <sheetName val="_Recovered_SheetName_102_"/>
-      <sheetName val="_Recovered_SheetName_103_"/>
-      <sheetName val="_Recovered_SheetName_104_"/>
-      <sheetName val="_Recovered_SheetName_105_"/>
-      <sheetName val="_Recovered_SheetName_106_"/>
-      <sheetName val="_Recovered_SheetName_107_"/>
-      <sheetName val="_Recovered_SheetName_108_"/>
-      <sheetName val="_Recovered_SheetName_109_"/>
-      <sheetName val="_Recovered_SheetName_110_"/>
-      <sheetName val="_Recovered_SheetName_111_"/>
-      <sheetName val="_Recovered_SheetName_112_"/>
-      <sheetName val="_Recovered_SheetName_113_"/>
-      <sheetName val="_Recovered_SheetName_114_"/>
-      <sheetName val="_Recovered_SheetName_115_"/>
-      <sheetName val="_Recovered_SheetName_116_"/>
-      <sheetName val="_Recovered_SheetName_117_"/>
-      <sheetName val="_Recovered_SheetName_118_"/>
-      <sheetName val="_Recovered_SheetName_119_"/>
-      <sheetName val="_Recovered_SheetName_120_"/>
-      <sheetName val="_Recovered_SheetName_121_"/>
-      <sheetName val="_Recovered_SheetName_122_"/>
-      <sheetName val="_Recovered_SheetName_123_"/>
-      <sheetName val="_Recovered_SheetName_124_"/>
-      <sheetName val="_Recovered_SheetName_125_"/>
-      <sheetName val="_Recovered_SheetName_126_"/>
-      <sheetName val="_Recovered_SheetName_127_"/>
-      <sheetName val="_Recovered_SheetName_128_"/>
-      <sheetName val="_Recovered_SheetName_129_"/>
-      <sheetName val="_Recovered_SheetName_130_"/>
-      <sheetName val="_Recovered_SheetName_131_"/>
-      <sheetName val="_Recovered_SheetName_132_"/>
-      <sheetName val="_Recovered_SheetName_133_"/>
-      <sheetName val="_Recovered_SheetName_134_"/>
-      <sheetName val="_Recovered_SheetName_135_"/>
-      <sheetName val="_Recovered_SheetName_136_"/>
-      <sheetName val="_Recovered_SheetName_137_"/>
-      <sheetName val="_Recovered_SheetName_138_"/>
-      <sheetName val="_Recovered_SheetName_139_"/>
-      <sheetName val="_Recovered_SheetName_140_"/>
-      <sheetName val="_Recovered_SheetName_141_"/>
-      <sheetName val="_Recovered_SheetName_142_"/>
-      <sheetName val="_Recovered_SheetName_143_"/>
-      <sheetName val="_Recovered_SheetName_144_"/>
-      <sheetName val="_Recovered_SheetName_145_"/>
-      <sheetName val="_Recovered_SheetName_146_"/>
-      <sheetName val="_Recovered_SheetName_147_"/>
-      <sheetName val="_Recovered_SheetName_148_"/>
-      <sheetName val="_Recovered_SheetName_149_"/>
-      <sheetName val="_Recovered_SheetName_150_"/>
-      <sheetName val="_Recovered_SheetName_151_"/>
-      <sheetName val="_Recovered_SheetName_152_"/>
-      <sheetName val="_Recovered_SheetName_153_"/>
-      <sheetName val="_Recovered_SheetName_154_"/>
-      <sheetName val="_Recovered_SheetName_155_"/>
-      <sheetName val="_Recovered_SheetName_156_"/>
-      <sheetName val="_Recovered_SheetName_157_"/>
-      <sheetName val="_Recovered_SheetName_158_"/>
-      <sheetName val="_Recovered_SheetName_159_"/>
-      <sheetName val="_Recovered_SheetName_160_"/>
-      <sheetName val="_Recovered_SheetName_161_"/>
-      <sheetName val="_Recovered_SheetName_162_"/>
-      <sheetName val="_Recovered_SheetName_163_"/>
-      <sheetName val="_Recovered_SheetName_164_"/>
-      <sheetName val="_Recovered_SheetName_165_"/>
-      <sheetName val="_Recovered_SheetName_166_"/>
-      <sheetName val="_Recovered_SheetName_167_"/>
-      <sheetName val="_Recovered_SheetName_168_"/>
-      <sheetName val="_Recovered_SheetName_169_"/>
-      <sheetName val="_Recovered_SheetName_170_"/>
-      <sheetName val="_Recovered_SheetName_171_"/>
-      <sheetName val="_Recovered_SheetName_172_"/>
-      <sheetName val="_Recovered_SheetName_173_"/>
-      <sheetName val="_Recovered_SheetName_174_"/>
-      <sheetName val="_Recovered_SheetName_175_"/>
-      <sheetName val="_Recovered_SheetName_176_"/>
-      <sheetName val="_Recovered_SheetName_177_"/>
-      <sheetName val="_Recovered_SheetName_178_"/>
-      <sheetName val="_Recovered_SheetName_179_"/>
-      <sheetName val="_Recovered_SheetName_180_"/>
-      <sheetName val="_Recovered_SheetName_181_"/>
-      <sheetName val="_Recovered_SheetName_182_"/>
-      <sheetName val="_Recovered_SheetName_183_"/>
-      <sheetName val="_Recovered_SheetName_184_"/>
-      <sheetName val="_Recovered_SheetName_185_"/>
-      <sheetName val="_Recovered_SheetName_186_"/>
-      <sheetName val="_Recovered_SheetName_187_"/>
-      <sheetName val="_Recovered_SheetName_188_"/>
-      <sheetName val="_Recovered_SheetName_189_"/>
-      <sheetName val="_Recovered_SheetName_190_"/>
-      <sheetName val="_Recovered_SheetName_191_"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_13"/>
-      <sheetName val="pow_(final)11"/>
-      <sheetName val="2cl_7x9_modified11"/>
-      <sheetName val="1cl_7x9_Ramon11"/>
-      <sheetName val="1cl_7x7_modified11"/>
-      <sheetName val="2cl_7x7_modified11"/>
-      <sheetName val="1cl_7x9_modified11"/>
-      <sheetName val="3cl_7x9_modified11"/>
-      <sheetName val="2sty4cl_11"/>
-      <sheetName val="2sty6cl_11"/>
-      <sheetName val="2sty8cl_11"/>
-      <sheetName val="h_e_11"/>
-      <sheetName val="cr_attached11"/>
-      <sheetName val="cr_detached11"/>
-      <sheetName val="rc_septic_vault11"/>
-      <sheetName val="chb_septic_vault11"/>
-      <sheetName val="1cl_(2)11"/>
-      <sheetName val="PROGRAM_of_WORK11"/>
-      <sheetName val="1cl_7x7_M11"/>
-      <sheetName val="repair_det_est2"/>
-      <sheetName val="program_of_works2"/>
-      <sheetName val="2cl_7x7_M2"/>
-      <sheetName val="3cl_7x7_M2"/>
-      <sheetName val="1cl_7x9_M2"/>
-      <sheetName val="2cl_7x9_M2"/>
-      <sheetName val="3cl_7x9_M2"/>
-      <sheetName val="4cl_7x9_M2"/>
-      <sheetName val="1cl_7x9_O2"/>
-      <sheetName val="2cl_7x9_O2"/>
-      <sheetName val="2cl_7x9_O_sphere2"/>
-      <sheetName val="3cl_7x9_O2"/>
-      <sheetName val="science_lab2"/>
-      <sheetName val="Typhoon_Resistance_2CL2"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_19"/>
-      <sheetName val="pow_(final)17"/>
-      <sheetName val="2cl_7x9_modified17"/>
-      <sheetName val="1cl_7x9_Ramon17"/>
-      <sheetName val="1cl_7x7_modified17"/>
-      <sheetName val="2cl_7x7_modified17"/>
-      <sheetName val="1cl_7x9_modified17"/>
-      <sheetName val="3cl_7x9_modified17"/>
-      <sheetName val="2sty4cl_17"/>
-      <sheetName val="2sty6cl_17"/>
-      <sheetName val="2sty8cl_17"/>
-      <sheetName val="h_e_17"/>
-      <sheetName val="cr_attached17"/>
-      <sheetName val="cr_detached17"/>
-      <sheetName val="rc_septic_vault17"/>
-      <sheetName val="chb_septic_vault17"/>
-      <sheetName val="1cl_(2)17"/>
-      <sheetName val="PROGRAM_of_WORK17"/>
-      <sheetName val="1cl_7x7_M17"/>
-      <sheetName val="repair_det_est8"/>
-      <sheetName val="program_of_works8"/>
-      <sheetName val="2cl_7x7_M8"/>
-      <sheetName val="3cl_7x7_M8"/>
-      <sheetName val="1cl_7x9_M8"/>
-      <sheetName val="2cl_7x9_M8"/>
-      <sheetName val="3cl_7x9_M8"/>
-      <sheetName val="4cl_7x9_M8"/>
-      <sheetName val="1cl_7x9_O8"/>
-      <sheetName val="2cl_7x9_O8"/>
-      <sheetName val="2cl_7x9_O_sphere8"/>
-      <sheetName val="3cl_7x9_O8"/>
-      <sheetName val="science_lab8"/>
-      <sheetName val="Typhoon_Resistance_2CL8"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_16"/>
-      <sheetName val="pow_(final)14"/>
-      <sheetName val="2cl_7x9_modified14"/>
-      <sheetName val="1cl_7x9_Ramon14"/>
-      <sheetName val="1cl_7x7_modified14"/>
-      <sheetName val="2cl_7x7_modified14"/>
-      <sheetName val="1cl_7x9_modified14"/>
-      <sheetName val="3cl_7x9_modified14"/>
-      <sheetName val="2sty4cl_14"/>
-      <sheetName val="2sty6cl_14"/>
-      <sheetName val="2sty8cl_14"/>
-      <sheetName val="h_e_14"/>
-      <sheetName val="cr_attached14"/>
-      <sheetName val="cr_detached14"/>
-      <sheetName val="rc_septic_vault14"/>
-      <sheetName val="chb_septic_vault14"/>
-      <sheetName val="1cl_(2)14"/>
-      <sheetName val="PROGRAM_of_WORK14"/>
-      <sheetName val="1cl_7x7_M14"/>
-      <sheetName val="repair_det_est5"/>
-      <sheetName val="program_of_works5"/>
-      <sheetName val="2cl_7x7_M5"/>
-      <sheetName val="3cl_7x7_M5"/>
-      <sheetName val="1cl_7x9_M5"/>
-      <sheetName val="2cl_7x9_M5"/>
-      <sheetName val="3cl_7x9_M5"/>
-      <sheetName val="4cl_7x9_M5"/>
-      <sheetName val="1cl_7x9_O5"/>
-      <sheetName val="2cl_7x9_O5"/>
-      <sheetName val="2cl_7x9_O_sphere5"/>
-      <sheetName val="3cl_7x9_O5"/>
-      <sheetName val="science_lab5"/>
-      <sheetName val="Typhoon_Resistance_2CL5"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_14"/>
-      <sheetName val="pow_(final)12"/>
-      <sheetName val="2cl_7x9_modified12"/>
-      <sheetName val="1cl_7x9_Ramon12"/>
-      <sheetName val="1cl_7x7_modified12"/>
-      <sheetName val="2cl_7x7_modified12"/>
-      <sheetName val="1cl_7x9_modified12"/>
-      <sheetName val="3cl_7x9_modified12"/>
-      <sheetName val="2sty4cl_12"/>
-      <sheetName val="2sty6cl_12"/>
-      <sheetName val="2sty8cl_12"/>
-      <sheetName val="h_e_12"/>
-      <sheetName val="cr_attached12"/>
-      <sheetName val="cr_detached12"/>
-      <sheetName val="rc_septic_vault12"/>
-      <sheetName val="chb_septic_vault12"/>
-      <sheetName val="1cl_(2)12"/>
-      <sheetName val="PROGRAM_of_WORK12"/>
-      <sheetName val="1cl_7x7_M12"/>
-      <sheetName val="repair_det_est3"/>
-      <sheetName val="program_of_works3"/>
-      <sheetName val="2cl_7x7_M3"/>
-      <sheetName val="3cl_7x7_M3"/>
-      <sheetName val="1cl_7x9_M3"/>
-      <sheetName val="2cl_7x9_M3"/>
-      <sheetName val="3cl_7x9_M3"/>
-      <sheetName val="4cl_7x9_M3"/>
-      <sheetName val="1cl_7x9_O3"/>
-      <sheetName val="2cl_7x9_O3"/>
-      <sheetName val="2cl_7x9_O_sphere3"/>
-      <sheetName val="3cl_7x9_O3"/>
-      <sheetName val="science_lab3"/>
-      <sheetName val="Typhoon_Resistance_2CL3"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_15"/>
-      <sheetName val="pow_(final)13"/>
-      <sheetName val="2cl_7x9_modified13"/>
-      <sheetName val="1cl_7x9_Ramon13"/>
-      <sheetName val="1cl_7x7_modified13"/>
-      <sheetName val="2cl_7x7_modified13"/>
-      <sheetName val="1cl_7x9_modified13"/>
-      <sheetName val="3cl_7x9_modified13"/>
-      <sheetName val="2sty4cl_13"/>
-      <sheetName val="2sty6cl_13"/>
-      <sheetName val="2sty8cl_13"/>
-      <sheetName val="h_e_13"/>
-      <sheetName val="cr_attached13"/>
-      <sheetName val="cr_detached13"/>
-      <sheetName val="rc_septic_vault13"/>
-      <sheetName val="chb_septic_vault13"/>
-      <sheetName val="1cl_(2)13"/>
-      <sheetName val="PROGRAM_of_WORK13"/>
-      <sheetName val="1cl_7x7_M13"/>
-      <sheetName val="repair_det_est4"/>
-      <sheetName val="program_of_works4"/>
-      <sheetName val="2cl_7x7_M4"/>
-      <sheetName val="3cl_7x7_M4"/>
-      <sheetName val="1cl_7x9_M4"/>
-      <sheetName val="2cl_7x9_M4"/>
-      <sheetName val="3cl_7x9_M4"/>
-      <sheetName val="4cl_7x9_M4"/>
-      <sheetName val="1cl_7x9_O4"/>
-      <sheetName val="2cl_7x9_O4"/>
-      <sheetName val="2cl_7x9_O_sphere4"/>
-      <sheetName val="3cl_7x9_O4"/>
-      <sheetName val="science_lab4"/>
-      <sheetName val="Typhoon_Resistance_2CL4"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_17"/>
-      <sheetName val="pow_(final)15"/>
-      <sheetName val="2cl_7x9_modified15"/>
-      <sheetName val="1cl_7x9_Ramon15"/>
-      <sheetName val="1cl_7x7_modified15"/>
-      <sheetName val="2cl_7x7_modified15"/>
-      <sheetName val="1cl_7x9_modified15"/>
-      <sheetName val="3cl_7x9_modified15"/>
-      <sheetName val="2sty4cl_15"/>
-      <sheetName val="2sty6cl_15"/>
-      <sheetName val="2sty8cl_15"/>
-      <sheetName val="h_e_15"/>
-      <sheetName val="cr_attached15"/>
-      <sheetName val="cr_detached15"/>
-      <sheetName val="rc_septic_vault15"/>
-      <sheetName val="chb_septic_vault15"/>
-      <sheetName val="1cl_(2)15"/>
-      <sheetName val="PROGRAM_of_WORK15"/>
-      <sheetName val="1cl_7x7_M15"/>
-      <sheetName val="repair_det_est6"/>
-      <sheetName val="program_of_works6"/>
-      <sheetName val="2cl_7x7_M6"/>
-      <sheetName val="3cl_7x7_M6"/>
-      <sheetName val="1cl_7x9_M6"/>
-      <sheetName val="2cl_7x9_M6"/>
-      <sheetName val="3cl_7x9_M6"/>
-      <sheetName val="4cl_7x9_M6"/>
-      <sheetName val="1cl_7x9_O6"/>
-      <sheetName val="2cl_7x9_O6"/>
-      <sheetName val="2cl_7x9_O_sphere6"/>
-      <sheetName val="3cl_7x9_O6"/>
-      <sheetName val="science_lab6"/>
-      <sheetName val="Typhoon_Resistance_2CL6"/>
-      <sheetName val="DECS_2cl_OMS_(2)5"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)5"/>
-      <sheetName val="DECS_2cl_OMS_(2)3"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)3"/>
-      <sheetName val="DECS_2cl_OMS_(2)1"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)1"/>
-      <sheetName val="DECS_2cl_OMS_(2)2"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)2"/>
-      <sheetName val="DECS_2cl_OMS_(2)4"/>
-      <sheetName val="COP2_okiot_tabuac_bcps(100)4"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_18"/>
-      <sheetName val="pow_(final)16"/>
-      <sheetName val="2cl_7x9_modified16"/>
-      <sheetName val="1cl_7x9_Ramon16"/>
-      <sheetName val="1cl_7x7_modified16"/>
-      <sheetName val="2cl_7x7_modified16"/>
-      <sheetName val="1cl_7x9_modified16"/>
-      <sheetName val="3cl_7x9_modified16"/>
-      <sheetName val="2sty4cl_16"/>
-      <sheetName val="2sty6cl_16"/>
-      <sheetName val="2sty8cl_16"/>
-      <sheetName val="h_e_16"/>
-      <sheetName val="cr_attached16"/>
-      <sheetName val="cr_detached16"/>
-      <sheetName val="rc_septic_vault16"/>
-      <sheetName val="chb_septic_vault16"/>
-      <sheetName val="1cl_(2)16"/>
-      <sheetName val="PROGRAM_of_WORK16"/>
-      <sheetName val="1cl_7x7_M16"/>
-      <sheetName val="repair_det_est7"/>
-      <sheetName val="program_of_works7"/>
-      <sheetName val="2cl_7x7_M7"/>
-      <sheetName val="3cl_7x7_M7"/>
-      <sheetName val="1cl_7x9_M7"/>
-      <sheetName val="2cl_7x9_M7"/>
-      <sheetName val="3cl_7x9_M7"/>
-      <sheetName val="4cl_7x9_M7"/>
-      <sheetName val="1cl_7x9_O7"/>
-      <sheetName val="2cl_7x9_O7"/>
-      <sheetName val="2cl_7x9_O_sphere7"/>
-      <sheetName val="3cl_7x9_O7"/>
-      <sheetName val="science_lab7"/>
-      <sheetName val="Typhoon_Resistance_2CL7"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_20"/>
-      <sheetName val="pow_(final)18"/>
-      <sheetName val="2cl_7x9_modified18"/>
-      <sheetName val="1cl_7x9_Ramon18"/>
-      <sheetName val="1cl_7x7_modified18"/>
-      <sheetName val="2cl_7x7_modified18"/>
-      <sheetName val="1cl_7x9_modified18"/>
-      <sheetName val="3cl_7x9_modified18"/>
-      <sheetName val="2sty4cl_18"/>
-      <sheetName val="2sty6cl_18"/>
-      <sheetName val="2sty8cl_18"/>
-      <sheetName val="h_e_18"/>
-      <sheetName val="cr_attached18"/>
-      <sheetName val="cr_detached18"/>
-      <sheetName val="rc_septic_vault18"/>
-      <sheetName val="chb_septic_vault18"/>
-      <sheetName val="1cl_(2)18"/>
-      <sheetName val="PROGRAM_of_WORK18"/>
-      <sheetName val="1cl_7x7_M18"/>
-      <sheetName val="repair_det_est9"/>
-      <sheetName val="program_of_works9"/>
-      <sheetName val="2cl_7x7_M9"/>
-      <sheetName val="3cl_7x7_M9"/>
-      <sheetName val="1cl_7x9_M9"/>
-      <sheetName val="2cl_7x9_M9"/>
-      <sheetName val="3cl_7x9_M9"/>
-      <sheetName val="4cl_7x9_M9"/>
-      <sheetName val="1cl_7x9_O9"/>
-      <sheetName val="2cl_7x9_O9"/>
-      <sheetName val="2cl_7x9_O_sphere9"/>
-      <sheetName val="3cl_7x9_O9"/>
-      <sheetName val="science_lab9"/>
-      <sheetName val="Typhoon_Resistance_2CL9"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_22"/>
-      <sheetName val="pow_(final)20"/>
-      <sheetName val="2cl_7x9_modified20"/>
-      <sheetName val="1cl_7x9_Ramon20"/>
-      <sheetName val="1cl_7x7_modified20"/>
-      <sheetName val="2cl_7x7_modified20"/>
-      <sheetName val="1cl_7x9_modified20"/>
-      <sheetName val="3cl_7x9_modified20"/>
-      <sheetName val="2sty4cl_20"/>
-      <sheetName val="2sty6cl_20"/>
-      <sheetName val="2sty8cl_20"/>
-      <sheetName val="h_e_20"/>
-      <sheetName val="cr_attached20"/>
-      <sheetName val="cr_detached20"/>
-      <sheetName val="rc_septic_vault20"/>
-      <sheetName val="chb_septic_vault20"/>
-      <sheetName val="1cl_(2)20"/>
-      <sheetName val="PROGRAM_of_WORK20"/>
-      <sheetName val="1cl_7x7_M20"/>
-      <sheetName val="repair_det_est11"/>
-      <sheetName val="program_of_works11"/>
-      <sheetName val="2cl_7x7_M11"/>
-      <sheetName val="3cl_7x7_M11"/>
-      <sheetName val="1cl_7x9_M11"/>
-      <sheetName val="2cl_7x9_M11"/>
-      <sheetName val="3cl_7x9_M11"/>
-      <sheetName val="4cl_7x9_M11"/>
-      <sheetName val="1cl_7x9_O11"/>
-      <sheetName val="2cl_7x9_O11"/>
-      <sheetName val="2cl_7x9_O_sphere11"/>
-      <sheetName val="3cl_7x9_O11"/>
-      <sheetName val="science_lab11"/>
-      <sheetName val="Typhoon_Resistance_2CL11"/>
-      <sheetName val="1cl_7x9_modified_wo_ceiling_21"/>
-      <sheetName val="pow_(final)19"/>
-      <sheetName val="2cl_7x9_modified19"/>
-      <sheetName val="1cl_7x9_Ramon19"/>
-      <sheetName val="1cl_7x7_modified19"/>
-      <sheetName val="2cl_7x7_modified19"/>
-      <sheetName val="1cl_7x9_modified19"/>
-      <sheetName val="3cl_7x9_modified19"/>
-      <sheetName val="2sty4cl_19"/>
-      <sheetName val="2sty6cl_19"/>
-      <sheetName val="2sty8cl_19"/>
-      <sheetName val="h_e_19"/>
-      <sheetName val="cr_attached19"/>
-      <sheetName val="cr_detached19"/>
-      <sheetName val="rc_septic_vault19"/>
-      <sheetName val="chb_septic_vault19"/>
-      <sheetName val="1cl_(2)19"/>
-      <sheetName val="PROGRAM_of_WORK19"/>
-      <sheetName val="1cl_7x7_M19"/>
-      <sheetName val="repair_det_est10"/>
-      <sheetName val="program_of_works10"/>
-      <sheetName val="2cl_7x7_M10"/>
-      <sheetName val="3cl_7x7_M10"/>
-      <sheetName val="1cl_7x9_M10"/>
-      <sheetName val="2cl_7x9_M10"/>
-      <sheetName val="3cl_7x9_M10"/>
-      <sheetName val="4cl_7x9_M10"/>
-      <sheetName val="1cl_7x9_O10"/>
-      <sheetName val="2cl_7x9_O10"/>
-      <sheetName val="2cl_7x9_O_sphere10"/>
-      <sheetName val="3cl_7x9_O10"/>
-      <sheetName val="science_lab10"/>
-      <sheetName val="Typhoon_Resistance_2CL10"/>
-      <sheetName val="Detailed_Estimate1"/>
-      <sheetName val="unit_weight_of_angle_bars1"/>
-      <sheetName val="unit_weight_of_purlins1"/>
-      <sheetName val="NEWCON_2017_(CL)1"/>
-      <sheetName val="BEFF_20161"/>
-      <sheetName val="Account_Type1"/>
-      <sheetName val="Source_of_data"/>
-      <sheetName val="⋜ú曆衟Ùꩋᄷ}衭_x0009_d駒ÿ꫏ì蠱"/>
-      <sheetName val="Costs and Types"/>
-      <sheetName val="GRAND SUM"/>
-      <sheetName val="Summary Conf Rm"/>
-      <sheetName val="DET CONF RM"/>
-      <sheetName val="rc ceptic vault"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39"/>
-      <sheetData sheetId="40"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-      <sheetData sheetId="59"/>
-      <sheetData sheetId="60"/>
-      <sheetData sheetId="61"/>
-      <sheetData sheetId="62"/>
-      <sheetData sheetId="63"/>
-      <sheetData sheetId="64"/>
-      <sheetData sheetId="65"/>
-      <sheetData sheetId="66"/>
-      <sheetData sheetId="67"/>
-      <sheetData sheetId="68"/>
-      <sheetData sheetId="69"/>
-      <sheetData sheetId="70"/>
-      <sheetData sheetId="71"/>
-      <sheetData sheetId="72"/>
-      <sheetData sheetId="73"/>
-      <sheetData sheetId="74"/>
-      <sheetData sheetId="75"/>
-      <sheetData sheetId="76"/>
-      <sheetData sheetId="77"/>
-      <sheetData sheetId="78"/>
-      <sheetData sheetId="79"/>
-      <sheetData sheetId="80"/>
-      <sheetData sheetId="81"/>
-      <sheetData sheetId="82"/>
-      <sheetData sheetId="83"/>
-      <sheetData sheetId="84"/>
-      <sheetData sheetId="85"/>
-      <sheetData sheetId="86"/>
-      <sheetData sheetId="87"/>
-      <sheetData sheetId="88"/>
-      <sheetData sheetId="89"/>
-      <sheetData sheetId="90"/>
-      <sheetData sheetId="91"/>
-      <sheetData sheetId="92"/>
-      <sheetData sheetId="93"/>
-      <sheetData sheetId="94"/>
-      <sheetData sheetId="95"/>
-      <sheetData sheetId="96"/>
-      <sheetData sheetId="97"/>
-      <sheetData sheetId="98"/>
-      <sheetData sheetId="99"/>
-      <sheetData sheetId="100"/>
-      <sheetData sheetId="101"/>
-      <sheetData sheetId="102"/>
-      <sheetData sheetId="103"/>
-      <sheetData sheetId="104"/>
-      <sheetData sheetId="105"/>
-      <sheetData sheetId="106"/>
-      <sheetData sheetId="107"/>
-      <sheetData sheetId="108"/>
-      <sheetData sheetId="109"/>
-      <sheetData sheetId="110"/>
-      <sheetData sheetId="111"/>
-      <sheetData sheetId="112"/>
-      <sheetData sheetId="113"/>
-      <sheetData sheetId="114"/>
-      <sheetData sheetId="115"/>
-      <sheetData sheetId="116"/>
-      <sheetData sheetId="117"/>
-      <sheetData sheetId="118"/>
-      <sheetData sheetId="119"/>
-      <sheetData sheetId="120"/>
-      <sheetData sheetId="121"/>
-      <sheetData sheetId="122"/>
-      <sheetData sheetId="123"/>
-      <sheetData sheetId="124"/>
-      <sheetData sheetId="125"/>
-      <sheetData sheetId="126"/>
-      <sheetData sheetId="127"/>
-      <sheetData sheetId="128"/>
-      <sheetData sheetId="129"/>
-      <sheetData sheetId="130"/>
-      <sheetData sheetId="131"/>
-      <sheetData sheetId="132"/>
-      <sheetData sheetId="133"/>
-      <sheetData sheetId="134"/>
-      <sheetData sheetId="135"/>
-      <sheetData sheetId="136"/>
-      <sheetData sheetId="137"/>
-      <sheetData sheetId="138"/>
-      <sheetData sheetId="139"/>
-      <sheetData sheetId="140"/>
-      <sheetData sheetId="141"/>
-      <sheetData sheetId="142"/>
-      <sheetData sheetId="143"/>
-      <sheetData sheetId="144"/>
-      <sheetData sheetId="145"/>
-      <sheetData sheetId="146"/>
-      <sheetData sheetId="147"/>
-      <sheetData sheetId="148"/>
-      <sheetData sheetId="149"/>
-      <sheetData sheetId="150"/>
-      <sheetData sheetId="151"/>
-      <sheetData sheetId="152"/>
-      <sheetData sheetId="153"/>
-      <sheetData sheetId="154"/>
-      <sheetData sheetId="155"/>
-      <sheetData sheetId="156"/>
-      <sheetData sheetId="157"/>
-      <sheetData sheetId="158"/>
-      <sheetData sheetId="159"/>
-      <sheetData sheetId="160"/>
-      <sheetData sheetId="161"/>
-      <sheetData sheetId="162"/>
-      <sheetData sheetId="163"/>
-      <sheetData sheetId="164"/>
-      <sheetData sheetId="165"/>
-      <sheetData sheetId="166"/>
-      <sheetData sheetId="167"/>
-      <sheetData sheetId="168"/>
-      <sheetData sheetId="169"/>
-      <sheetData sheetId="170"/>
-      <sheetData sheetId="171"/>
-      <sheetData sheetId="172"/>
-      <sheetData sheetId="173"/>
-      <sheetData sheetId="174"/>
-      <sheetData sheetId="175"/>
-      <sheetData sheetId="176"/>
-      <sheetData sheetId="177"/>
-      <sheetData sheetId="178"/>
-      <sheetData sheetId="179"/>
-      <sheetData sheetId="180"/>
-      <sheetData sheetId="181"/>
-      <sheetData sheetId="182"/>
-      <sheetData sheetId="183"/>
-      <sheetData sheetId="184"/>
-      <sheetData sheetId="185"/>
-      <sheetData sheetId="186"/>
-      <sheetData sheetId="187"/>
-      <sheetData sheetId="188"/>
-      <sheetData sheetId="189"/>
-      <sheetData sheetId="190"/>
-      <sheetData sheetId="191"/>
-      <sheetData sheetId="192"/>
-      <sheetData sheetId="193"/>
-      <sheetData sheetId="194"/>
-      <sheetData sheetId="195"/>
-      <sheetData sheetId="196"/>
-      <sheetData sheetId="197"/>
-      <sheetData sheetId="198"/>
-      <sheetData sheetId="199"/>
-      <sheetData sheetId="200"/>
-      <sheetData sheetId="201"/>
-      <sheetData sheetId="202"/>
-      <sheetData sheetId="203"/>
-      <sheetData sheetId="204"/>
-      <sheetData sheetId="205"/>
-      <sheetData sheetId="206"/>
-      <sheetData sheetId="207"/>
-      <sheetData sheetId="208" refreshError="1"/>
-      <sheetData sheetId="209"/>
-      <sheetData sheetId="210"/>
-      <sheetData sheetId="211"/>
-      <sheetData sheetId="212"/>
-      <sheetData sheetId="213"/>
-      <sheetData sheetId="214"/>
-      <sheetData sheetId="215"/>
-      <sheetData sheetId="216"/>
-      <sheetData sheetId="217"/>
-      <sheetData sheetId="218"/>
-      <sheetData sheetId="219"/>
-      <sheetData sheetId="220"/>
-      <sheetData sheetId="221"/>
-      <sheetData sheetId="222"/>
-      <sheetData sheetId="223"/>
-      <sheetData sheetId="224"/>
-      <sheetData sheetId="225"/>
-      <sheetData sheetId="226"/>
-      <sheetData sheetId="227"/>
-      <sheetData sheetId="228"/>
-      <sheetData sheetId="229"/>
-      <sheetData sheetId="230"/>
-      <sheetData sheetId="231"/>
-      <sheetData sheetId="232"/>
-      <sheetData sheetId="233"/>
-      <sheetData sheetId="234"/>
-      <sheetData sheetId="235"/>
-      <sheetData sheetId="236"/>
-      <sheetData sheetId="237"/>
-      <sheetData sheetId="238"/>
-      <sheetData sheetId="239" refreshError="1"/>
-      <sheetData sheetId="240" refreshError="1"/>
-      <sheetData sheetId="241" refreshError="1"/>
-      <sheetData sheetId="242"/>
-      <sheetData sheetId="243"/>
-      <sheetData sheetId="244" refreshError="1"/>
-      <sheetData sheetId="245"/>
-      <sheetData sheetId="246"/>
-      <sheetData sheetId="247"/>
-      <sheetData sheetId="248"/>
-      <sheetData sheetId="249"/>
-      <sheetData sheetId="250"/>
-      <sheetData sheetId="251"/>
-      <sheetData sheetId="252"/>
-      <sheetData sheetId="253"/>
-      <sheetData sheetId="254"/>
-      <sheetData sheetId="255"/>
-      <sheetData sheetId="256" refreshError="1"/>
-      <sheetData sheetId="257" refreshError="1"/>
-      <sheetData sheetId="258" refreshError="1"/>
-      <sheetData sheetId="259" refreshError="1"/>
-      <sheetData sheetId="260" refreshError="1"/>
-      <sheetData sheetId="261" refreshError="1"/>
-      <sheetData sheetId="262" refreshError="1"/>
-      <sheetData sheetId="263" refreshError="1"/>
-      <sheetData sheetId="264" refreshError="1"/>
-      <sheetData sheetId="265" refreshError="1"/>
-      <sheetData sheetId="266" refreshError="1"/>
-      <sheetData sheetId="267" refreshError="1"/>
-      <sheetData sheetId="268" refreshError="1"/>
-      <sheetData sheetId="269" refreshError="1"/>
-      <sheetData sheetId="270" refreshError="1"/>
-      <sheetData sheetId="271" refreshError="1"/>
-      <sheetData sheetId="272" refreshError="1"/>
-      <sheetData sheetId="273" refreshError="1"/>
-      <sheetData sheetId="274" refreshError="1"/>
-      <sheetData sheetId="275" refreshError="1"/>
-      <sheetData sheetId="276" refreshError="1"/>
-      <sheetData sheetId="277" refreshError="1"/>
-      <sheetData sheetId="278" refreshError="1"/>
-      <sheetData sheetId="279" refreshError="1"/>
-      <sheetData sheetId="280" refreshError="1"/>
-      <sheetData sheetId="281" refreshError="1"/>
-      <sheetData sheetId="282" refreshError="1"/>
-      <sheetData sheetId="283" refreshError="1"/>
-      <sheetData sheetId="284" refreshError="1"/>
-      <sheetData sheetId="285" refreshError="1"/>
-      <sheetData sheetId="286" refreshError="1"/>
-      <sheetData sheetId="287" refreshError="1"/>
-      <sheetData sheetId="288" refreshError="1"/>
-      <sheetData sheetId="289" refreshError="1"/>
-      <sheetData sheetId="290" refreshError="1"/>
-      <sheetData sheetId="291" refreshError="1"/>
-      <sheetData sheetId="292" refreshError="1"/>
-      <sheetData sheetId="293" refreshError="1"/>
-      <sheetData sheetId="294" refreshError="1"/>
-      <sheetData sheetId="295" refreshError="1"/>
-      <sheetData sheetId="296" refreshError="1"/>
-      <sheetData sheetId="297" refreshError="1"/>
-      <sheetData sheetId="298" refreshError="1"/>
-      <sheetData sheetId="299" refreshError="1"/>
-      <sheetData sheetId="300" refreshError="1"/>
-      <sheetData sheetId="301" refreshError="1"/>
-      <sheetData sheetId="302" refreshError="1"/>
-      <sheetData sheetId="303" refreshError="1"/>
-      <sheetData sheetId="304" refreshError="1"/>
-      <sheetData sheetId="305" refreshError="1"/>
-      <sheetData sheetId="306" refreshError="1"/>
-      <sheetData sheetId="307" refreshError="1"/>
-      <sheetData sheetId="308" refreshError="1"/>
-      <sheetData sheetId="309" refreshError="1"/>
-      <sheetData sheetId="310" refreshError="1"/>
-      <sheetData sheetId="311" refreshError="1"/>
-      <sheetData sheetId="312" refreshError="1"/>
-      <sheetData sheetId="313" refreshError="1"/>
-      <sheetData sheetId="314" refreshError="1"/>
-      <sheetData sheetId="315" refreshError="1"/>
-      <sheetData sheetId="316" refreshError="1"/>
-      <sheetData sheetId="317" refreshError="1"/>
-      <sheetData sheetId="318" refreshError="1"/>
-      <sheetData sheetId="319" refreshError="1"/>
-      <sheetData sheetId="320" refreshError="1"/>
-      <sheetData sheetId="321" refreshError="1"/>
-      <sheetData sheetId="322" refreshError="1"/>
-      <sheetData sheetId="323" refreshError="1"/>
-      <sheetData sheetId="324" refreshError="1"/>
-      <sheetData sheetId="325" refreshError="1"/>
-      <sheetData sheetId="326" refreshError="1"/>
-      <sheetData sheetId="327" refreshError="1"/>
-      <sheetData sheetId="328" refreshError="1"/>
-      <sheetData sheetId="329" refreshError="1"/>
-      <sheetData sheetId="330" refreshError="1"/>
-      <sheetData sheetId="331" refreshError="1"/>
-      <sheetData sheetId="332" refreshError="1"/>
-      <sheetData sheetId="333" refreshError="1"/>
-      <sheetData sheetId="334" refreshError="1"/>
-      <sheetData sheetId="335" refreshError="1"/>
-      <sheetData sheetId="336" refreshError="1"/>
-      <sheetData sheetId="337" refreshError="1"/>
-      <sheetData sheetId="338" refreshError="1"/>
-      <sheetData sheetId="339" refreshError="1"/>
-      <sheetData sheetId="340" refreshError="1"/>
-      <sheetData sheetId="341" refreshError="1"/>
-      <sheetData sheetId="342" refreshError="1"/>
-      <sheetData sheetId="343" refreshError="1"/>
-      <sheetData sheetId="344" refreshError="1"/>
-      <sheetData sheetId="345" refreshError="1"/>
-      <sheetData sheetId="346" refreshError="1"/>
-      <sheetData sheetId="347" refreshError="1"/>
-      <sheetData sheetId="348" refreshError="1"/>
-      <sheetData sheetId="349" refreshError="1"/>
-      <sheetData sheetId="350" refreshError="1"/>
-      <sheetData sheetId="351" refreshError="1"/>
-      <sheetData sheetId="352" refreshError="1"/>
-      <sheetData sheetId="353" refreshError="1"/>
-      <sheetData sheetId="354" refreshError="1"/>
-      <sheetData sheetId="355" refreshError="1"/>
-      <sheetData sheetId="356" refreshError="1"/>
-      <sheetData sheetId="357" refreshError="1"/>
-      <sheetData sheetId="358" refreshError="1"/>
-      <sheetData sheetId="359" refreshError="1"/>
-      <sheetData sheetId="360" refreshError="1"/>
-      <sheetData sheetId="361" refreshError="1"/>
-      <sheetData sheetId="362" refreshError="1"/>
-      <sheetData sheetId="363" refreshError="1"/>
-      <sheetData sheetId="364" refreshError="1"/>
-      <sheetData sheetId="365" refreshError="1"/>
-      <sheetData sheetId="366" refreshError="1"/>
-      <sheetData sheetId="367" refreshError="1"/>
-      <sheetData sheetId="368" refreshError="1"/>
-      <sheetData sheetId="369" refreshError="1"/>
-      <sheetData sheetId="370" refreshError="1"/>
-      <sheetData sheetId="371" refreshError="1"/>
-      <sheetData sheetId="372" refreshError="1"/>
-      <sheetData sheetId="373" refreshError="1"/>
-      <sheetData sheetId="374" refreshError="1"/>
-      <sheetData sheetId="375" refreshError="1"/>
-      <sheetData sheetId="376" refreshError="1"/>
-      <sheetData sheetId="377" refreshError="1"/>
-      <sheetData sheetId="378" refreshError="1"/>
-      <sheetData sheetId="379" refreshError="1"/>
-      <sheetData sheetId="380" refreshError="1"/>
-      <sheetData sheetId="381" refreshError="1"/>
-      <sheetData sheetId="382" refreshError="1"/>
-      <sheetData sheetId="383" refreshError="1"/>
-      <sheetData sheetId="384" refreshError="1"/>
-      <sheetData sheetId="385" refreshError="1"/>
-      <sheetData sheetId="386" refreshError="1"/>
-      <sheetData sheetId="387" refreshError="1"/>
-      <sheetData sheetId="388" refreshError="1"/>
-      <sheetData sheetId="389" refreshError="1"/>
-      <sheetData sheetId="390" refreshError="1"/>
-      <sheetData sheetId="391" refreshError="1"/>
-      <sheetData sheetId="392" refreshError="1"/>
-      <sheetData sheetId="393" refreshError="1"/>
-      <sheetData sheetId="394" refreshError="1"/>
-      <sheetData sheetId="395" refreshError="1"/>
-      <sheetData sheetId="396" refreshError="1"/>
-      <sheetData sheetId="397" refreshError="1"/>
-      <sheetData sheetId="398" refreshError="1"/>
-      <sheetData sheetId="399" refreshError="1"/>
-      <sheetData sheetId="400" refreshError="1"/>
-      <sheetData sheetId="401" refreshError="1"/>
-      <sheetData sheetId="402" refreshError="1"/>
-      <sheetData sheetId="403" refreshError="1"/>
-      <sheetData sheetId="404" refreshError="1"/>
-      <sheetData sheetId="405" refreshError="1"/>
-      <sheetData sheetId="406" refreshError="1"/>
-      <sheetData sheetId="407" refreshError="1"/>
-      <sheetData sheetId="408" refreshError="1"/>
-      <sheetData sheetId="409" refreshError="1"/>
-      <sheetData sheetId="410" refreshError="1"/>
-      <sheetData sheetId="411" refreshError="1"/>
-      <sheetData sheetId="412" refreshError="1"/>
-      <sheetData sheetId="413" refreshError="1"/>
-      <sheetData sheetId="414" refreshError="1"/>
-      <sheetData sheetId="415" refreshError="1"/>
-      <sheetData sheetId="416" refreshError="1"/>
-      <sheetData sheetId="417" refreshError="1"/>
-      <sheetData sheetId="418" refreshError="1"/>
-      <sheetData sheetId="419" refreshError="1"/>
-      <sheetData sheetId="420" refreshError="1"/>
-      <sheetData sheetId="421" refreshError="1"/>
-      <sheetData sheetId="422" refreshError="1"/>
-      <sheetData sheetId="423" refreshError="1"/>
-      <sheetData sheetId="424" refreshError="1"/>
-      <sheetData sheetId="425" refreshError="1"/>
-      <sheetData sheetId="426" refreshError="1"/>
-      <sheetData sheetId="427" refreshError="1"/>
-      <sheetData sheetId="428" refreshError="1"/>
-      <sheetData sheetId="429" refreshError="1"/>
-      <sheetData sheetId="430" refreshError="1"/>
-      <sheetData sheetId="431"/>
-      <sheetData sheetId="432"/>
-      <sheetData sheetId="433"/>
-      <sheetData sheetId="434"/>
-      <sheetData sheetId="435"/>
-      <sheetData sheetId="436"/>
-      <sheetData sheetId="437"/>
-      <sheetData sheetId="438"/>
-      <sheetData sheetId="439"/>
-      <sheetData sheetId="440"/>
-      <sheetData sheetId="441"/>
-      <sheetData sheetId="442"/>
-      <sheetData sheetId="443"/>
-      <sheetData sheetId="444"/>
-      <sheetData sheetId="445"/>
-      <sheetData sheetId="446"/>
-      <sheetData sheetId="447"/>
-      <sheetData sheetId="448"/>
-      <sheetData sheetId="449"/>
-      <sheetData sheetId="450"/>
-      <sheetData sheetId="451"/>
-      <sheetData sheetId="452"/>
-      <sheetData sheetId="453"/>
-      <sheetData sheetId="454"/>
-      <sheetData sheetId="455"/>
-      <sheetData sheetId="456"/>
-      <sheetData sheetId="457"/>
-      <sheetData sheetId="458"/>
-      <sheetData sheetId="459"/>
-      <sheetData sheetId="460"/>
-      <sheetData sheetId="461"/>
-      <sheetData sheetId="462"/>
-      <sheetData sheetId="463"/>
-      <sheetData sheetId="464"/>
-      <sheetData sheetId="465"/>
-      <sheetData sheetId="466"/>
-      <sheetData sheetId="467"/>
-      <sheetData sheetId="468"/>
-      <sheetData sheetId="469"/>
-      <sheetData sheetId="470"/>
-      <sheetData sheetId="471"/>
-      <sheetData sheetId="472"/>
-      <sheetData sheetId="473"/>
-      <sheetData sheetId="474"/>
-      <sheetData sheetId="475"/>
-      <sheetData sheetId="476"/>
-      <sheetData sheetId="477"/>
-      <sheetData sheetId="478"/>
-      <sheetData sheetId="479"/>
-      <sheetData sheetId="480"/>
-      <sheetData sheetId="481"/>
-      <sheetData sheetId="482"/>
-      <sheetData sheetId="483"/>
-      <sheetData sheetId="484"/>
-      <sheetData sheetId="485"/>
-      <sheetData sheetId="486"/>
-      <sheetData sheetId="487"/>
-      <sheetData sheetId="488"/>
-      <sheetData sheetId="489"/>
-      <sheetData sheetId="490"/>
-      <sheetData sheetId="491"/>
-      <sheetData sheetId="492"/>
-      <sheetData sheetId="493"/>
-      <sheetData sheetId="494"/>
-      <sheetData sheetId="495"/>
-      <sheetData sheetId="496"/>
-      <sheetData sheetId="497"/>
-      <sheetData sheetId="498"/>
-      <sheetData sheetId="499"/>
-      <sheetData sheetId="500"/>
-      <sheetData sheetId="501"/>
-      <sheetData sheetId="502"/>
-      <sheetData sheetId="503"/>
-      <sheetData sheetId="504"/>
-      <sheetData sheetId="505"/>
-      <sheetData sheetId="506"/>
-      <sheetData sheetId="507"/>
-      <sheetData sheetId="508"/>
-      <sheetData sheetId="509"/>
-      <sheetData sheetId="510"/>
-      <sheetData sheetId="511"/>
-      <sheetData sheetId="512"/>
-      <sheetData sheetId="513"/>
-      <sheetData sheetId="514"/>
-      <sheetData sheetId="515"/>
-      <sheetData sheetId="516"/>
-      <sheetData sheetId="517"/>
-      <sheetData sheetId="518"/>
-      <sheetData sheetId="519"/>
-      <sheetData sheetId="520"/>
-      <sheetData sheetId="521"/>
-      <sheetData sheetId="522"/>
-      <sheetData sheetId="523"/>
-      <sheetData sheetId="524"/>
-      <sheetData sheetId="525"/>
-      <sheetData sheetId="526"/>
-      <sheetData sheetId="527"/>
-      <sheetData sheetId="528"/>
-      <sheetData sheetId="529"/>
-      <sheetData sheetId="530"/>
-      <sheetData sheetId="531"/>
-      <sheetData sheetId="532"/>
-      <sheetData sheetId="533"/>
-      <sheetData sheetId="534"/>
-      <sheetData sheetId="535"/>
-      <sheetData sheetId="536"/>
-      <sheetData sheetId="537"/>
-      <sheetData sheetId="538"/>
-      <sheetData sheetId="539"/>
-      <sheetData sheetId="540"/>
-      <sheetData sheetId="541"/>
-      <sheetData sheetId="542"/>
-      <sheetData sheetId="543"/>
-      <sheetData sheetId="544"/>
-      <sheetData sheetId="545"/>
-      <sheetData sheetId="546"/>
-      <sheetData sheetId="547"/>
-      <sheetData sheetId="548"/>
-      <sheetData sheetId="549"/>
-      <sheetData sheetId="550"/>
-      <sheetData sheetId="551"/>
-      <sheetData sheetId="552"/>
-      <sheetData sheetId="553"/>
-      <sheetData sheetId="554"/>
-      <sheetData sheetId="555"/>
-      <sheetData sheetId="556"/>
-      <sheetData sheetId="557"/>
-      <sheetData sheetId="558"/>
-      <sheetData sheetId="559"/>
-      <sheetData sheetId="560"/>
-      <sheetData sheetId="561"/>
-      <sheetData sheetId="562"/>
-      <sheetData sheetId="563"/>
-      <sheetData sheetId="564"/>
-      <sheetData sheetId="565"/>
-      <sheetData sheetId="566"/>
-      <sheetData sheetId="567"/>
-      <sheetData sheetId="568"/>
-      <sheetData sheetId="569"/>
-      <sheetData sheetId="570"/>
-      <sheetData sheetId="571"/>
-      <sheetData sheetId="572"/>
-      <sheetData sheetId="573"/>
-      <sheetData sheetId="574"/>
-      <sheetData sheetId="575"/>
-      <sheetData sheetId="576"/>
-      <sheetData sheetId="577"/>
-      <sheetData sheetId="578"/>
-      <sheetData sheetId="579"/>
-      <sheetData sheetId="580"/>
-      <sheetData sheetId="581"/>
-      <sheetData sheetId="582"/>
-      <sheetData sheetId="583"/>
-      <sheetData sheetId="584"/>
-      <sheetData sheetId="585"/>
-      <sheetData sheetId="586"/>
-      <sheetData sheetId="587"/>
-      <sheetData sheetId="588"/>
-      <sheetData sheetId="589"/>
-      <sheetData sheetId="590"/>
-      <sheetData sheetId="591"/>
-      <sheetData sheetId="592"/>
-      <sheetData sheetId="593"/>
-      <sheetData sheetId="594"/>
-      <sheetData sheetId="595"/>
-      <sheetData sheetId="596"/>
-      <sheetData sheetId="597"/>
-      <sheetData sheetId="598"/>
-      <sheetData sheetId="599"/>
-      <sheetData sheetId="600"/>
-      <sheetData sheetId="601"/>
-      <sheetData sheetId="602"/>
-      <sheetData sheetId="603"/>
-      <sheetData sheetId="604"/>
-      <sheetData sheetId="605"/>
-      <sheetData sheetId="606"/>
-      <sheetData sheetId="607"/>
-      <sheetData sheetId="608"/>
-      <sheetData sheetId="609"/>
-      <sheetData sheetId="610"/>
-      <sheetData sheetId="611"/>
-      <sheetData sheetId="612"/>
-      <sheetData sheetId="613"/>
-      <sheetData sheetId="614"/>
-      <sheetData sheetId="615"/>
-      <sheetData sheetId="616"/>
-      <sheetData sheetId="617"/>
-      <sheetData sheetId="618"/>
-      <sheetData sheetId="619"/>
-      <sheetData sheetId="620"/>
-      <sheetData sheetId="621"/>
-      <sheetData sheetId="622"/>
-      <sheetData sheetId="623"/>
-      <sheetData sheetId="624"/>
-      <sheetData sheetId="625"/>
-      <sheetData sheetId="626"/>
-      <sheetData sheetId="627"/>
-      <sheetData sheetId="628"/>
-      <sheetData sheetId="629"/>
-      <sheetData sheetId="630"/>
-      <sheetData sheetId="631"/>
-      <sheetData sheetId="632"/>
-      <sheetData sheetId="633"/>
-      <sheetData sheetId="634"/>
-      <sheetData sheetId="635"/>
-      <sheetData sheetId="636"/>
-      <sheetData sheetId="637"/>
-      <sheetData sheetId="638"/>
-      <sheetData sheetId="639"/>
-      <sheetData sheetId="640"/>
-      <sheetData sheetId="641"/>
-      <sheetData sheetId="642"/>
-      <sheetData sheetId="643"/>
-      <sheetData sheetId="644"/>
-      <sheetData sheetId="645"/>
-      <sheetData sheetId="646"/>
-      <sheetData sheetId="647"/>
-      <sheetData sheetId="648"/>
-      <sheetData sheetId="649"/>
-      <sheetData sheetId="650"/>
-      <sheetData sheetId="651"/>
-      <sheetData sheetId="652"/>
-      <sheetData sheetId="653"/>
-      <sheetData sheetId="654"/>
-      <sheetData sheetId="655"/>
-      <sheetData sheetId="656"/>
-      <sheetData sheetId="657"/>
-      <sheetData sheetId="658"/>
-      <sheetData sheetId="659"/>
-      <sheetData sheetId="660"/>
-      <sheetData sheetId="661"/>
-      <sheetData sheetId="662"/>
-      <sheetData sheetId="663"/>
-      <sheetData sheetId="664"/>
-      <sheetData sheetId="665"/>
-      <sheetData sheetId="666"/>
-      <sheetData sheetId="667"/>
-      <sheetData sheetId="668"/>
-      <sheetData sheetId="669"/>
-      <sheetData sheetId="670"/>
-      <sheetData sheetId="671"/>
-      <sheetData sheetId="672"/>
-      <sheetData sheetId="673"/>
-      <sheetData sheetId="674"/>
-      <sheetData sheetId="675"/>
-      <sheetData sheetId="676"/>
-      <sheetData sheetId="677"/>
-      <sheetData sheetId="678"/>
-      <sheetData sheetId="679"/>
-      <sheetData sheetId="680"/>
-      <sheetData sheetId="681"/>
-      <sheetData sheetId="682"/>
-      <sheetData sheetId="683"/>
-      <sheetData sheetId="684"/>
-      <sheetData sheetId="685"/>
-      <sheetData sheetId="686"/>
-      <sheetData sheetId="687"/>
-      <sheetData sheetId="688"/>
-      <sheetData sheetId="689"/>
-      <sheetData sheetId="690"/>
-      <sheetData sheetId="691"/>
-      <sheetData sheetId="692"/>
-      <sheetData sheetId="693"/>
-      <sheetData sheetId="694"/>
-      <sheetData sheetId="695"/>
-      <sheetData sheetId="696"/>
-      <sheetData sheetId="697"/>
-      <sheetData sheetId="698"/>
-      <sheetData sheetId="699"/>
-      <sheetData sheetId="700"/>
-      <sheetData sheetId="701"/>
-      <sheetData sheetId="702"/>
-      <sheetData sheetId="703"/>
-      <sheetData sheetId="704"/>
-      <sheetData sheetId="705"/>
-      <sheetData sheetId="706"/>
-      <sheetData sheetId="707"/>
-      <sheetData sheetId="708"/>
-      <sheetData sheetId="709"/>
-      <sheetData sheetId="710"/>
-      <sheetData sheetId="711"/>
-      <sheetData sheetId="712"/>
-      <sheetData sheetId="713"/>
-      <sheetData sheetId="714"/>
-      <sheetData sheetId="715"/>
-      <sheetData sheetId="716"/>
-      <sheetData sheetId="717"/>
-      <sheetData sheetId="718"/>
-      <sheetData sheetId="719"/>
-      <sheetData sheetId="720"/>
-      <sheetData sheetId="721"/>
-      <sheetData sheetId="722"/>
-      <sheetData sheetId="723"/>
-      <sheetData sheetId="724"/>
-      <sheetData sheetId="725"/>
-      <sheetData sheetId="726"/>
-      <sheetData sheetId="727"/>
-      <sheetData sheetId="728"/>
-      <sheetData sheetId="729"/>
-      <sheetData sheetId="730"/>
-      <sheetData sheetId="731"/>
-      <sheetData sheetId="732"/>
-      <sheetData sheetId="733"/>
-      <sheetData sheetId="734"/>
-      <sheetData sheetId="735"/>
-      <sheetData sheetId="736"/>
-      <sheetData sheetId="737"/>
-      <sheetData sheetId="738"/>
-      <sheetData sheetId="739"/>
-      <sheetData sheetId="740"/>
-      <sheetData sheetId="741"/>
-      <sheetData sheetId="742"/>
-      <sheetData sheetId="743"/>
-      <sheetData sheetId="744"/>
-      <sheetData sheetId="745"/>
-      <sheetData sheetId="746"/>
-      <sheetData sheetId="747"/>
-      <sheetData sheetId="748"/>
-      <sheetData sheetId="749"/>
-      <sheetData sheetId="750"/>
-      <sheetData sheetId="751"/>
-      <sheetData sheetId="752"/>
-      <sheetData sheetId="753"/>
-      <sheetData sheetId="754"/>
-      <sheetData sheetId="755"/>
-      <sheetData sheetId="756"/>
-      <sheetData sheetId="757"/>
-      <sheetData sheetId="758"/>
-      <sheetData sheetId="759"/>
-      <sheetData sheetId="760"/>
-      <sheetData sheetId="761"/>
-      <sheetData sheetId="762"/>
-      <sheetData sheetId="763"/>
-      <sheetData sheetId="764"/>
-      <sheetData sheetId="765"/>
-      <sheetData sheetId="766"/>
-      <sheetData sheetId="767"/>
-      <sheetData sheetId="768"/>
-      <sheetData sheetId="769"/>
-      <sheetData sheetId="770"/>
-      <sheetData sheetId="771"/>
-      <sheetData sheetId="772"/>
-      <sheetData sheetId="773"/>
-      <sheetData sheetId="774"/>
-      <sheetData sheetId="775"/>
-      <sheetData sheetId="776"/>
-      <sheetData sheetId="777"/>
-      <sheetData sheetId="778" refreshError="1"/>
-      <sheetData sheetId="779" refreshError="1"/>
-      <sheetData sheetId="780" refreshError="1"/>
-      <sheetData sheetId="781" refreshError="1"/>
-      <sheetData sheetId="782" refreshError="1"/>
-      <sheetData sheetId="783" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -2664,7 +970,6 @@
       <sheetName val="ALOBS"/>
       <sheetName val="Edu-5"/>
       <sheetName val="LYDS4 (2)"/>
-      <sheetName val="Database"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -2676,13 +981,12 @@
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
-      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink11.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4385,7 +2689,136 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink12.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="summary"/>
+      <sheetName val="Graceano Lopez"/>
+      <sheetName val="Ernesto Rondon HS"/>
+      <sheetName val="Juan Luna ES"/>
+      <sheetName val="Pamplona ES"/>
+      <sheetName val="Ilaya ES"/>
+      <sheetName val="Ernesto Rondon HS (2)"/>
+      <sheetName val="RESPSCI"/>
+      <sheetName val="Paranaque NHS"/>
+      <sheetName val="Talon ES"/>
+      <sheetName val="Zapote ES"/>
+      <sheetName val="Quantity Take-off"/>
+      <sheetName val="Graceano Lopez Jaena ES"/>
+      <sheetName val="A. Albert ES"/>
+      <sheetName val="Las Pinas HS (CAA)"/>
+      <sheetName val="Database"/>
+      <sheetName val="Graceano_Lopez2"/>
+      <sheetName val="Ernesto_Rondon_HS2"/>
+      <sheetName val="Juan_Luna_ES2"/>
+      <sheetName val="Pamplona_ES2"/>
+      <sheetName val="Ilaya_ES2"/>
+      <sheetName val="Ernesto_Rondon_HS_(2)2"/>
+      <sheetName val="Paranaque_NHS2"/>
+      <sheetName val="Talon_ES2"/>
+      <sheetName val="Zapote_ES2"/>
+      <sheetName val="Quantity_Take-off2"/>
+      <sheetName val="Graceano_Lopez_Jaena_ES2"/>
+      <sheetName val="A__Albert_ES2"/>
+      <sheetName val="Las_Pinas_HS_(CAA)2"/>
+      <sheetName val="Graceano_Lopez"/>
+      <sheetName val="Ernesto_Rondon_HS"/>
+      <sheetName val="Juan_Luna_ES"/>
+      <sheetName val="Pamplona_ES"/>
+      <sheetName val="Ilaya_ES"/>
+      <sheetName val="Ernesto_Rondon_HS_(2)"/>
+      <sheetName val="Paranaque_NHS"/>
+      <sheetName val="Talon_ES"/>
+      <sheetName val="Zapote_ES"/>
+      <sheetName val="Quantity_Take-off"/>
+      <sheetName val="Graceano_Lopez_Jaena_ES"/>
+      <sheetName val="A__Albert_ES"/>
+      <sheetName val="Las_Pinas_HS_(CAA)"/>
+      <sheetName val="Graceano_Lopez1"/>
+      <sheetName val="Ernesto_Rondon_HS1"/>
+      <sheetName val="Juan_Luna_ES1"/>
+      <sheetName val="Pamplona_ES1"/>
+      <sheetName val="Ilaya_ES1"/>
+      <sheetName val="Ernesto_Rondon_HS_(2)1"/>
+      <sheetName val="Paranaque_NHS1"/>
+      <sheetName val="Talon_ES1"/>
+      <sheetName val="Zapote_ES1"/>
+      <sheetName val="Quantity_Take-off1"/>
+      <sheetName val="Graceano_Lopez_Jaena_ES1"/>
+      <sheetName val="A__Albert_ES1"/>
+      <sheetName val="Las_Pinas_HS_(CAA)1"/>
+      <sheetName val="Contractor"/>
+      <sheetName val="DECS 2cl OMS (2)"/>
+      <sheetName val="buhelebongES"/>
+      <sheetName val="Max"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34" refreshError="1"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43" refreshError="1"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
+      <sheetData sheetId="47" refreshError="1"/>
+      <sheetData sheetId="48" refreshError="1"/>
+      <sheetData sheetId="49" refreshError="1"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink13.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4466,7 +2899,140 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink14.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="POW"/>
+      <sheetName val="Lupang Pangako"/>
+      <sheetName val="Database"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet3"/>
+      <sheetName val="SUMMARY"/>
+      <sheetName val="Lupang_Pangako"/>
+      <sheetName val="Max"/>
+      <sheetName val="Lupang_Pangako6"/>
+      <sheetName val="Lupang_Pangako1"/>
+      <sheetName val="Lupang_Pangako4"/>
+      <sheetName val="Lupang_Pangako2"/>
+      <sheetName val="Lupang_Pangako3"/>
+      <sheetName val="Lupang_Pangako5"/>
+      <sheetName val="Lupang_Pangako7"/>
+      <sheetName val="Lupang_Pangako8"/>
+      <sheetName val="Lupang_Pangako10"/>
+      <sheetName val="Lupang_Pangako9"/>
+      <sheetName val="Target for 2019"/>
+      <sheetName val="Per Program"/>
+      <sheetName val="REPAIR 2017"/>
+      <sheetName val="Repair 2018"/>
+      <sheetName val="REPAIR 2019"/>
+      <sheetName val="Electrification 2018"/>
+      <sheetName val="buhelebongES"/>
+      <sheetName val="EDU4"/>
+      <sheetName val="dbase"/>
+      <sheetName val="Lupang_Pangako11"/>
+      <sheetName val="Target_for_2019"/>
+      <sheetName val="Per_Program"/>
+      <sheetName val="REPAIR_2017"/>
+      <sheetName val="Repair_2018"/>
+      <sheetName val="REPAIR_2019"/>
+      <sheetName val="Electrification_2018"/>
+      <sheetName val="SOM"/>
+      <sheetName val="DO 71 s 2013"/>
+      <sheetName val="LIBRARY"/>
+      <sheetName val="101(2)e"/>
+      <sheetName val="101(2)g"/>
+      <sheetName val="101(2)c"/>
+      <sheetName val="101(2)f"/>
+      <sheetName val="Worksheet"/>
+      <sheetName val="Lupang_Pangako12"/>
+      <sheetName val="Target_for_20191"/>
+      <sheetName val="Per_Program1"/>
+      <sheetName val="REPAIR_20171"/>
+      <sheetName val="Repair_20181"/>
+      <sheetName val="REPAIR_20191"/>
+      <sheetName val="Electrification_20181"/>
+      <sheetName val="rates"/>
+      <sheetName val="RATE"/>
+      <sheetName val="ABC"/>
+      <sheetName val="general"/>
+      <sheetName val="ACCOMP. REPORT sub"/>
+      <sheetName val="TABLES"/>
+      <sheetName val="DRSB_Weight"/>
+      <sheetName val="EQUIPMENT"/>
+      <sheetName val="nm"/>
+      <sheetName val="Payitems"/>
+      <sheetName val="Basis (2)"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
+      <sheetData sheetId="32"/>
+      <sheetData sheetId="33"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35" refreshError="1"/>
+      <sheetData sheetId="36" refreshError="1"/>
+      <sheetData sheetId="37" refreshError="1"/>
+      <sheetData sheetId="38" refreshError="1"/>
+      <sheetData sheetId="39" refreshError="1"/>
+      <sheetData sheetId="40" refreshError="1"/>
+      <sheetData sheetId="41" refreshError="1"/>
+      <sheetData sheetId="42" refreshError="1"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50" refreshError="1"/>
+      <sheetData sheetId="51" refreshError="1"/>
+      <sheetData sheetId="52" refreshError="1"/>
+      <sheetData sheetId="53" refreshError="1"/>
+      <sheetData sheetId="54" refreshError="1"/>
+      <sheetData sheetId="55" refreshError="1"/>
+      <sheetData sheetId="56" refreshError="1"/>
+      <sheetData sheetId="57" refreshError="1"/>
+      <sheetData sheetId="58" refreshError="1"/>
+      <sheetData sheetId="59" refreshError="1"/>
+      <sheetData sheetId="60" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink15.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4485,7 +3051,120 @@
 </externalLink>
 </file>
 
+<file path=xl/externalLinks/externalLink16.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Enrolees&amp;Graduated"/>
+      <sheetName val="Classrooms"/>
+      <sheetName val="Drop-out"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink17.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="SchInfo"/>
+      <sheetName val="Table1"/>
+      <sheetName val="Tables2-3"/>
+      <sheetName val="Tables4-5"/>
+      <sheetName val="Table6"/>
+      <sheetName val="Table7"/>
+      <sheetName val="Table8"/>
+      <sheetName val="Tables9-10"/>
+      <sheetName val="Table11"/>
+      <sheetName val="Table12"/>
+      <sheetName val="Table13-Box1"/>
+      <sheetName val="Tables15"/>
+      <sheetName val="Box2-Table16"/>
+      <sheetName val="Box3"/>
+      <sheetName val="Tables17-18"/>
+      <sheetName val="Box4-5"/>
+      <sheetName val="Tables19-20"/>
+      <sheetName val="Box6-Table21"/>
+      <sheetName val="Table22-Box8"/>
+      <sheetName val="Boxes9-11"/>
+      <sheetName val="Table23-Box12"/>
+      <sheetName val="Boxes13-14"/>
+      <sheetName val="Alloc working w formula"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Enrolees&amp;Graduated"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="EDU4"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="EDU4"/>
+      <sheetName val="edu May -ot"/>
+      <sheetName val="LYDS4"/>
+      <sheetName val="MIMAY4"/>
+      <sheetName val="HELEN4"/>
+      <sheetName val="OT-PAYROLL"/>
+      <sheetName val="ALOBS"/>
+      <sheetName val="Edu-5"/>
+      <sheetName val="LYDS4 (2)"/>
+      <sheetName val="Database"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4510,7 +3189,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -4529,7 +3208,1605 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="PRIORITY 2"/>
+      <sheetName val="PRIORITY 3"/>
+      <sheetName val="Costs and Types"/>
+      <sheetName val="Database"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Liminangcong"/>
+      <sheetName val="Recommendation"/>
+      <sheetName val="Liminangcong-SWA"/>
+      <sheetName val="Liminangcong-WPR"/>
+      <sheetName val="Database"/>
+      <sheetName val="Template"/>
+      <sheetName val="Summary"/>
+      <sheetName val="DataInput"/>
+      <sheetName val="1cl 7x9 modified wo ceiling "/>
+      <sheetName val="pow (final)"/>
+      <sheetName val="2cl 7x9 modified"/>
+      <sheetName val="1cl 7x9 Ramon"/>
+      <sheetName val="1cl 7x7 modified"/>
+      <sheetName val="2cl 7x7 modified"/>
+      <sheetName val="dbase"/>
+      <sheetName val="industrial"/>
+      <sheetName val="1cl 7x9 modified"/>
+      <sheetName val="3cl 7x9 modified"/>
+      <sheetName val="1cl"/>
+      <sheetName val="2cl"/>
+      <sheetName val="3cl"/>
+      <sheetName val="5cl"/>
+      <sheetName val="2sty4cl "/>
+      <sheetName val="2sty6cl "/>
+      <sheetName val="2sty8cl "/>
+      <sheetName val="3sty9cl"/>
+      <sheetName val="h.e."/>
+      <sheetName val="cr attached"/>
+      <sheetName val="cr detached"/>
+      <sheetName val="rc septic vault"/>
+      <sheetName val="chb septic vault"/>
+      <sheetName val="1cl (2)"/>
+      <sheetName val="PROGRAM of WORK"/>
+      <sheetName val="1cl 7x7 M"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_5"/>
+      <sheetName val="pow_(final)5"/>
+      <sheetName val="2cl_7x9_modified5"/>
+      <sheetName val="1cl_7x9_Ramon5"/>
+      <sheetName val="1cl_7x7_modified5"/>
+      <sheetName val="2cl_7x7_modified5"/>
+      <sheetName val="1cl_7x9_modified5"/>
+      <sheetName val="3cl_7x9_modified5"/>
+      <sheetName val="2sty4cl_5"/>
+      <sheetName val="2sty6cl_5"/>
+      <sheetName val="2sty8cl_5"/>
+      <sheetName val="h_e_5"/>
+      <sheetName val="cr_attached5"/>
+      <sheetName val="cr_detached5"/>
+      <sheetName val="rc_septic_vault5"/>
+      <sheetName val="chb_septic_vault5"/>
+      <sheetName val="1cl_(2)5"/>
+      <sheetName val="PROGRAM_of_WORK5"/>
+      <sheetName val="1cl_7x7_M5"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_"/>
+      <sheetName val="pow_(final)"/>
+      <sheetName val="2cl_7x9_modified"/>
+      <sheetName val="1cl_7x9_Ramon"/>
+      <sheetName val="1cl_7x7_modified"/>
+      <sheetName val="2cl_7x7_modified"/>
+      <sheetName val="1cl_7x9_modified"/>
+      <sheetName val="3cl_7x9_modified"/>
+      <sheetName val="2sty4cl_"/>
+      <sheetName val="2sty6cl_"/>
+      <sheetName val="2sty8cl_"/>
+      <sheetName val="h_e_"/>
+      <sheetName val="cr_attached"/>
+      <sheetName val="cr_detached"/>
+      <sheetName val="rc_septic_vault"/>
+      <sheetName val="chb_septic_vault"/>
+      <sheetName val="1cl_(2)"/>
+      <sheetName val="PROGRAM_of_WORK"/>
+      <sheetName val="1cl_7x7_M"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_1"/>
+      <sheetName val="pow_(final)1"/>
+      <sheetName val="2cl_7x9_modified1"/>
+      <sheetName val="1cl_7x9_Ramon1"/>
+      <sheetName val="1cl_7x7_modified1"/>
+      <sheetName val="2cl_7x7_modified1"/>
+      <sheetName val="1cl_7x9_modified1"/>
+      <sheetName val="3cl_7x9_modified1"/>
+      <sheetName val="2sty4cl_1"/>
+      <sheetName val="2sty6cl_1"/>
+      <sheetName val="2sty8cl_1"/>
+      <sheetName val="h_e_1"/>
+      <sheetName val="cr_attached1"/>
+      <sheetName val="cr_detached1"/>
+      <sheetName val="rc_septic_vault1"/>
+      <sheetName val="chb_septic_vault1"/>
+      <sheetName val="1cl_(2)1"/>
+      <sheetName val="PROGRAM_of_WORK1"/>
+      <sheetName val="1cl_7x7_M1"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_3"/>
+      <sheetName val="pow_(final)3"/>
+      <sheetName val="2cl_7x9_modified3"/>
+      <sheetName val="1cl_7x9_Ramon3"/>
+      <sheetName val="1cl_7x7_modified3"/>
+      <sheetName val="2cl_7x7_modified3"/>
+      <sheetName val="1cl_7x9_modified3"/>
+      <sheetName val="3cl_7x9_modified3"/>
+      <sheetName val="2sty4cl_3"/>
+      <sheetName val="2sty6cl_3"/>
+      <sheetName val="2sty8cl_3"/>
+      <sheetName val="h_e_3"/>
+      <sheetName val="cr_attached3"/>
+      <sheetName val="cr_detached3"/>
+      <sheetName val="rc_septic_vault3"/>
+      <sheetName val="chb_septic_vault3"/>
+      <sheetName val="1cl_(2)3"/>
+      <sheetName val="PROGRAM_of_WORK3"/>
+      <sheetName val="1cl_7x7_M3"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_2"/>
+      <sheetName val="pow_(final)2"/>
+      <sheetName val="2cl_7x9_modified2"/>
+      <sheetName val="1cl_7x9_Ramon2"/>
+      <sheetName val="1cl_7x7_modified2"/>
+      <sheetName val="2cl_7x7_modified2"/>
+      <sheetName val="1cl_7x9_modified2"/>
+      <sheetName val="3cl_7x9_modified2"/>
+      <sheetName val="2sty4cl_2"/>
+      <sheetName val="2sty6cl_2"/>
+      <sheetName val="2sty8cl_2"/>
+      <sheetName val="h_e_2"/>
+      <sheetName val="cr_attached2"/>
+      <sheetName val="cr_detached2"/>
+      <sheetName val="rc_septic_vault2"/>
+      <sheetName val="chb_septic_vault2"/>
+      <sheetName val="1cl_(2)2"/>
+      <sheetName val="PROGRAM_of_WORK2"/>
+      <sheetName val="1cl_7x7_M2"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_4"/>
+      <sheetName val="pow_(final)4"/>
+      <sheetName val="2cl_7x9_modified4"/>
+      <sheetName val="1cl_7x9_Ramon4"/>
+      <sheetName val="1cl_7x7_modified4"/>
+      <sheetName val="2cl_7x7_modified4"/>
+      <sheetName val="1cl_7x9_modified4"/>
+      <sheetName val="3cl_7x9_modified4"/>
+      <sheetName val="2sty4cl_4"/>
+      <sheetName val="2sty6cl_4"/>
+      <sheetName val="2sty8cl_4"/>
+      <sheetName val="h_e_4"/>
+      <sheetName val="cr_attached4"/>
+      <sheetName val="cr_detached4"/>
+      <sheetName val="rc_septic_vault4"/>
+      <sheetName val="chb_septic_vault4"/>
+      <sheetName val="1cl_(2)4"/>
+      <sheetName val="PROGRAM_of_WORK4"/>
+      <sheetName val="1cl_7x7_M4"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_6"/>
+      <sheetName val="pow_(final)6"/>
+      <sheetName val="2cl_7x9_modified6"/>
+      <sheetName val="1cl_7x9_Ramon6"/>
+      <sheetName val="1cl_7x7_modified6"/>
+      <sheetName val="2cl_7x7_modified6"/>
+      <sheetName val="1cl_7x9_modified6"/>
+      <sheetName val="3cl_7x9_modified6"/>
+      <sheetName val="2sty4cl_6"/>
+      <sheetName val="2sty6cl_6"/>
+      <sheetName val="2sty8cl_6"/>
+      <sheetName val="h_e_6"/>
+      <sheetName val="cr_attached6"/>
+      <sheetName val="cr_detached6"/>
+      <sheetName val="rc_septic_vault6"/>
+      <sheetName val="chb_septic_vault6"/>
+      <sheetName val="1cl_(2)6"/>
+      <sheetName val="PROGRAM_of_WORK6"/>
+      <sheetName val="1cl_7x7_M6"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_7"/>
+      <sheetName val="pow_(final)7"/>
+      <sheetName val="2cl_7x9_modified7"/>
+      <sheetName val="1cl_7x9_Ramon7"/>
+      <sheetName val="1cl_7x7_modified7"/>
+      <sheetName val="2cl_7x7_modified7"/>
+      <sheetName val="1cl_7x9_modified7"/>
+      <sheetName val="3cl_7x9_modified7"/>
+      <sheetName val="2sty4cl_7"/>
+      <sheetName val="2sty6cl_7"/>
+      <sheetName val="2sty8cl_7"/>
+      <sheetName val="h_e_7"/>
+      <sheetName val="cr_attached7"/>
+      <sheetName val="cr_detached7"/>
+      <sheetName val="rc_septic_vault7"/>
+      <sheetName val="chb_septic_vault7"/>
+      <sheetName val="1cl_(2)7"/>
+      <sheetName val="PROGRAM_of_WORK7"/>
+      <sheetName val="1cl_7x7_M7"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_8"/>
+      <sheetName val="pow_(final)8"/>
+      <sheetName val="2cl_7x9_modified8"/>
+      <sheetName val="1cl_7x9_Ramon8"/>
+      <sheetName val="1cl_7x7_modified8"/>
+      <sheetName val="2cl_7x7_modified8"/>
+      <sheetName val="1cl_7x9_modified8"/>
+      <sheetName val="3cl_7x9_modified8"/>
+      <sheetName val="2sty4cl_8"/>
+      <sheetName val="2sty6cl_8"/>
+      <sheetName val="2sty8cl_8"/>
+      <sheetName val="h_e_8"/>
+      <sheetName val="cr_attached8"/>
+      <sheetName val="cr_detached8"/>
+      <sheetName val="rc_septic_vault8"/>
+      <sheetName val="chb_septic_vault8"/>
+      <sheetName val="1cl_(2)8"/>
+      <sheetName val="PROGRAM_of_WORK8"/>
+      <sheetName val="1cl_7x7_M8"/>
+      <sheetName val="POW"/>
+      <sheetName val="repair det est"/>
+      <sheetName val="program of works"/>
+      <sheetName val="2cl 7x7 M"/>
+      <sheetName val="3cl 7x7 M"/>
+      <sheetName val="1cl 7x9 M"/>
+      <sheetName val="2cl 7x9 M"/>
+      <sheetName val="3cl 7x9 M"/>
+      <sheetName val="4cl 7x9 M"/>
+      <sheetName val="1cl 7x9 O"/>
+      <sheetName val="2cl 7x9 O"/>
+      <sheetName val="2cl 7x9 O_sphere"/>
+      <sheetName val="3cl 7x9 O"/>
+      <sheetName val="multipurpose"/>
+      <sheetName val="science lab"/>
+      <sheetName val="Typhoon Resistance_2CL"/>
+      <sheetName val="RC_SV"/>
+      <sheetName val="CHB_SV"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_9"/>
+      <sheetName val="pow_(final)9"/>
+      <sheetName val="2cl_7x9_modified9"/>
+      <sheetName val="1cl_7x9_Ramon9"/>
+      <sheetName val="1cl_7x7_modified9"/>
+      <sheetName val="2cl_7x7_modified9"/>
+      <sheetName val="1cl_7x9_modified9"/>
+      <sheetName val="3cl_7x9_modified9"/>
+      <sheetName val="2sty4cl_9"/>
+      <sheetName val="2sty6cl_9"/>
+      <sheetName val="2sty8cl_9"/>
+      <sheetName val="h_e_9"/>
+      <sheetName val="cr_attached9"/>
+      <sheetName val="cr_detached9"/>
+      <sheetName val="rc_septic_vault9"/>
+      <sheetName val="chb_septic_vault9"/>
+      <sheetName val="1cl_(2)9"/>
+      <sheetName val="PROGRAM_of_WORK9"/>
+      <sheetName val="1cl_7x7_M9"/>
+      <sheetName val="repair_det_est"/>
+      <sheetName val="program_of_works"/>
+      <sheetName val="2cl_7x7_M"/>
+      <sheetName val="3cl_7x7_M"/>
+      <sheetName val="1cl_7x9_M"/>
+      <sheetName val="2cl_7x9_M"/>
+      <sheetName val="3cl_7x9_M"/>
+      <sheetName val="4cl_7x9_M"/>
+      <sheetName val="1cl_7x9_O"/>
+      <sheetName val="2cl_7x9_O"/>
+      <sheetName val="2cl_7x9_O_sphere"/>
+      <sheetName val="3cl_7x9_O"/>
+      <sheetName val="science_lab"/>
+      <sheetName val="Typhoon_Resistance_2CL"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_10"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_11"/>
+      <sheetName val="3sty15cl-1"/>
+      <sheetName val="buhelebongES"/>
+      <sheetName val="DECS 2cl OMS (2)"/>
+      <sheetName val="COP2 okiot tabuac bcps(100)"/>
+      <sheetName val="Detailed Estimate"/>
+      <sheetName val="Sheet2"/>
+      <sheetName val="Sheet1"/>
+      <sheetName val="unit weight of angle bars"/>
+      <sheetName val="unit weight of purlins"/>
+      <sheetName val="NEWCON 2017 (CL)"/>
+      <sheetName val="BEFF 2016"/>
+      <sheetName val="Account Type"/>
+      <sheetName val="Source of data"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_12"/>
+      <sheetName val="pow_(final)10"/>
+      <sheetName val="2cl_7x9_modified10"/>
+      <sheetName val="1cl_7x9_Ramon10"/>
+      <sheetName val="1cl_7x7_modified10"/>
+      <sheetName val="2cl_7x7_modified10"/>
+      <sheetName val="1cl_7x9_modified10"/>
+      <sheetName val="3cl_7x9_modified10"/>
+      <sheetName val="2sty4cl_10"/>
+      <sheetName val="2sty6cl_10"/>
+      <sheetName val="2sty8cl_10"/>
+      <sheetName val="h_e_10"/>
+      <sheetName val="cr_attached10"/>
+      <sheetName val="cr_detached10"/>
+      <sheetName val="rc_septic_vault10"/>
+      <sheetName val="chb_septic_vault10"/>
+      <sheetName val="1cl_(2)10"/>
+      <sheetName val="PROGRAM_of_WORK10"/>
+      <sheetName val="1cl_7x7_M10"/>
+      <sheetName val="repair_det_est1"/>
+      <sheetName val="program_of_works1"/>
+      <sheetName val="2cl_7x7_M1"/>
+      <sheetName val="3cl_7x7_M1"/>
+      <sheetName val="1cl_7x9_M1"/>
+      <sheetName val="2cl_7x9_M1"/>
+      <sheetName val="3cl_7x9_M1"/>
+      <sheetName val="4cl_7x9_M1"/>
+      <sheetName val="1cl_7x9_O1"/>
+      <sheetName val="2cl_7x9_O1"/>
+      <sheetName val="2cl_7x9_O_sphere1"/>
+      <sheetName val="3cl_7x9_O1"/>
+      <sheetName val="science_lab1"/>
+      <sheetName val="Typhoon_Resistance_2CL1"/>
+      <sheetName val="DECS_2cl_OMS_(2)"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)"/>
+      <sheetName val="Detailed_Estimate"/>
+      <sheetName val="unit_weight_of_angle_bars"/>
+      <sheetName val="unit_weight_of_purlins"/>
+      <sheetName val="NEWCON_2017_(CL)"/>
+      <sheetName val="BEFF_2016"/>
+      <sheetName val="Account_Type"/>
+      <sheetName val="900b"/>
+      <sheetName val="900a"/>
+      <sheetName val="1cl_7x9_Ramn1"/>
+      <sheetName val="⊹≣駤_≚7≎≭믧ì⋡뭦ꫭ⋬餱"/>
+      <sheetName val="⋜ú曆衟Ùꩋᄷ}衭 d駒ÿ꫏ì蠱"/>
+      <sheetName val="1_x0005_"/>
+      <sheetName val="_Recovered_SheetName_79_"/>
+      <sheetName val="_Recovered_SheetName_80_"/>
+      <sheetName val="_Recovered_SheetName_81_"/>
+      <sheetName val="_Recovered_SheetName_82_"/>
+      <sheetName val="_Recovered_SheetName_83_"/>
+      <sheetName val="_Recovered_SheetName_84_"/>
+      <sheetName val="_Recovered_SheetName_85_"/>
+      <sheetName val="_Recovered_SheetName_86_"/>
+      <sheetName val="_Recovered_SheetName_87_"/>
+      <sheetName val="_Recovered_SheetName_88_"/>
+      <sheetName val="_Recovered_SheetName_89_"/>
+      <sheetName val="_Recovered_SheetName_90_"/>
+      <sheetName val="_Recovered_SheetName_91_"/>
+      <sheetName val="_Recovered_SheetName_92_"/>
+      <sheetName val="_Recovered_SheetName_93_"/>
+      <sheetName val="_Recovered_SheetName_94_"/>
+      <sheetName val="_Recovered_SheetName_95_"/>
+      <sheetName val="_Recovered_SheetName_96_"/>
+      <sheetName val="_Recovered_SheetName_97_"/>
+      <sheetName val="_Recovered_SheetName_98_"/>
+      <sheetName val="_Recovered_SheetName_99_"/>
+      <sheetName val="_Recovered_SheetName_100_"/>
+      <sheetName val="_Recovered_SheetName_101_"/>
+      <sheetName val="_Recovered_SheetName_102_"/>
+      <sheetName val="_Recovered_SheetName_103_"/>
+      <sheetName val="_Recovered_SheetName_104_"/>
+      <sheetName val="_Recovered_SheetName_105_"/>
+      <sheetName val="_Recovered_SheetName_106_"/>
+      <sheetName val="_Recovered_SheetName_107_"/>
+      <sheetName val="_Recovered_SheetName_108_"/>
+      <sheetName val="_Recovered_SheetName_109_"/>
+      <sheetName val="_Recovered_SheetName_110_"/>
+      <sheetName val="_Recovered_SheetName_111_"/>
+      <sheetName val="_Recovered_SheetName_112_"/>
+      <sheetName val="_Recovered_SheetName_113_"/>
+      <sheetName val="_Recovered_SheetName_114_"/>
+      <sheetName val="_Recovered_SheetName_115_"/>
+      <sheetName val="_Recovered_SheetName_116_"/>
+      <sheetName val="_Recovered_SheetName_117_"/>
+      <sheetName val="_Recovered_SheetName_118_"/>
+      <sheetName val="_Recovered_SheetName_119_"/>
+      <sheetName val="_Recovered_SheetName_120_"/>
+      <sheetName val="_Recovered_SheetName_121_"/>
+      <sheetName val="_Recovered_SheetName_122_"/>
+      <sheetName val="_Recovered_SheetName_123_"/>
+      <sheetName val="_Recovered_SheetName_124_"/>
+      <sheetName val="_Recovered_SheetName_125_"/>
+      <sheetName val="_Recovered_SheetName_126_"/>
+      <sheetName val="_Recovered_SheetName_127_"/>
+      <sheetName val="_Recovered_SheetName_128_"/>
+      <sheetName val="_Recovered_SheetName_129_"/>
+      <sheetName val="_Recovered_SheetName_130_"/>
+      <sheetName val="_Recovered_SheetName_131_"/>
+      <sheetName val="_Recovered_SheetName_132_"/>
+      <sheetName val="_Recovered_SheetName_133_"/>
+      <sheetName val="_Recovered_SheetName_134_"/>
+      <sheetName val="_Recovered_SheetName_135_"/>
+      <sheetName val="_Recovered_SheetName_136_"/>
+      <sheetName val="_Recovered_SheetName_137_"/>
+      <sheetName val="_Recovered_SheetName_138_"/>
+      <sheetName val="_Recovered_SheetName_139_"/>
+      <sheetName val="_Recovered_SheetName_140_"/>
+      <sheetName val="_Recovered_SheetName_141_"/>
+      <sheetName val="_Recovered_SheetName_142_"/>
+      <sheetName val="_Recovered_SheetName_143_"/>
+      <sheetName val="_Recovered_SheetName_144_"/>
+      <sheetName val="_Recovered_SheetName_145_"/>
+      <sheetName val="_Recovered_SheetName_146_"/>
+      <sheetName val="_Recovered_SheetName_147_"/>
+      <sheetName val="_Recovered_SheetName_148_"/>
+      <sheetName val="_Recovered_SheetName_149_"/>
+      <sheetName val="_Recovered_SheetName_150_"/>
+      <sheetName val="_Recovered_SheetName_151_"/>
+      <sheetName val="_Recovered_SheetName_152_"/>
+      <sheetName val="_Recovered_SheetName_153_"/>
+      <sheetName val="_Recovered_SheetName_154_"/>
+      <sheetName val="_Recovered_SheetName_155_"/>
+      <sheetName val="_Recovered_SheetName_156_"/>
+      <sheetName val="_Recovered_SheetName_157_"/>
+      <sheetName val="_Recovered_SheetName_158_"/>
+      <sheetName val="_Recovered_SheetName_159_"/>
+      <sheetName val="_Recovered_SheetName_160_"/>
+      <sheetName val="_Recovered_SheetName_161_"/>
+      <sheetName val="_Recovered_SheetName_162_"/>
+      <sheetName val="_Recovered_SheetName_163_"/>
+      <sheetName val="_Recovered_SheetName_164_"/>
+      <sheetName val="_Recovered_SheetName_165_"/>
+      <sheetName val="_Recovered_SheetName_166_"/>
+      <sheetName val="_Recovered_SheetName_167_"/>
+      <sheetName val="_Recovered_SheetName_168_"/>
+      <sheetName val="_Recovered_SheetName_169_"/>
+      <sheetName val="_Recovered_SheetName_170_"/>
+      <sheetName val="_Recovered_SheetName_171_"/>
+      <sheetName val="_Recovered_SheetName_172_"/>
+      <sheetName val="_Recovered_SheetName_173_"/>
+      <sheetName val="_Recovered_SheetName_174_"/>
+      <sheetName val="_Recovered_SheetName_175_"/>
+      <sheetName val="_Recovered_SheetName_176_"/>
+      <sheetName val="_Recovered_SheetName_177_"/>
+      <sheetName val="_Recovered_SheetName_178_"/>
+      <sheetName val="_Recovered_SheetName_179_"/>
+      <sheetName val="_Recovered_SheetName_180_"/>
+      <sheetName val="_Recovered_SheetName_181_"/>
+      <sheetName val="_Recovered_SheetName_182_"/>
+      <sheetName val="_Recovered_SheetName_183_"/>
+      <sheetName val="_Recovered_SheetName_184_"/>
+      <sheetName val="_Recovered_SheetName_185_"/>
+      <sheetName val="_Recovered_SheetName_186_"/>
+      <sheetName val="_Recovered_SheetName_187_"/>
+      <sheetName val="_Recovered_SheetName_188_"/>
+      <sheetName val="_Recovered_SheetName_189_"/>
+      <sheetName val="_Recovered_SheetName_190_"/>
+      <sheetName val="_Recovered_SheetName_191_"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_13"/>
+      <sheetName val="pow_(final)11"/>
+      <sheetName val="2cl_7x9_modified11"/>
+      <sheetName val="1cl_7x9_Ramon11"/>
+      <sheetName val="1cl_7x7_modified11"/>
+      <sheetName val="2cl_7x7_modified11"/>
+      <sheetName val="1cl_7x9_modified11"/>
+      <sheetName val="3cl_7x9_modified11"/>
+      <sheetName val="2sty4cl_11"/>
+      <sheetName val="2sty6cl_11"/>
+      <sheetName val="2sty8cl_11"/>
+      <sheetName val="h_e_11"/>
+      <sheetName val="cr_attached11"/>
+      <sheetName val="cr_detached11"/>
+      <sheetName val="rc_septic_vault11"/>
+      <sheetName val="chb_septic_vault11"/>
+      <sheetName val="1cl_(2)11"/>
+      <sheetName val="PROGRAM_of_WORK11"/>
+      <sheetName val="1cl_7x7_M11"/>
+      <sheetName val="repair_det_est2"/>
+      <sheetName val="program_of_works2"/>
+      <sheetName val="2cl_7x7_M2"/>
+      <sheetName val="3cl_7x7_M2"/>
+      <sheetName val="1cl_7x9_M2"/>
+      <sheetName val="2cl_7x9_M2"/>
+      <sheetName val="3cl_7x9_M2"/>
+      <sheetName val="4cl_7x9_M2"/>
+      <sheetName val="1cl_7x9_O2"/>
+      <sheetName val="2cl_7x9_O2"/>
+      <sheetName val="2cl_7x9_O_sphere2"/>
+      <sheetName val="3cl_7x9_O2"/>
+      <sheetName val="science_lab2"/>
+      <sheetName val="Typhoon_Resistance_2CL2"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_19"/>
+      <sheetName val="pow_(final)17"/>
+      <sheetName val="2cl_7x9_modified17"/>
+      <sheetName val="1cl_7x9_Ramon17"/>
+      <sheetName val="1cl_7x7_modified17"/>
+      <sheetName val="2cl_7x7_modified17"/>
+      <sheetName val="1cl_7x9_modified17"/>
+      <sheetName val="3cl_7x9_modified17"/>
+      <sheetName val="2sty4cl_17"/>
+      <sheetName val="2sty6cl_17"/>
+      <sheetName val="2sty8cl_17"/>
+      <sheetName val="h_e_17"/>
+      <sheetName val="cr_attached17"/>
+      <sheetName val="cr_detached17"/>
+      <sheetName val="rc_septic_vault17"/>
+      <sheetName val="chb_septic_vault17"/>
+      <sheetName val="1cl_(2)17"/>
+      <sheetName val="PROGRAM_of_WORK17"/>
+      <sheetName val="1cl_7x7_M17"/>
+      <sheetName val="repair_det_est8"/>
+      <sheetName val="program_of_works8"/>
+      <sheetName val="2cl_7x7_M8"/>
+      <sheetName val="3cl_7x7_M8"/>
+      <sheetName val="1cl_7x9_M8"/>
+      <sheetName val="2cl_7x9_M8"/>
+      <sheetName val="3cl_7x9_M8"/>
+      <sheetName val="4cl_7x9_M8"/>
+      <sheetName val="1cl_7x9_O8"/>
+      <sheetName val="2cl_7x9_O8"/>
+      <sheetName val="2cl_7x9_O_sphere8"/>
+      <sheetName val="3cl_7x9_O8"/>
+      <sheetName val="science_lab8"/>
+      <sheetName val="Typhoon_Resistance_2CL8"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_16"/>
+      <sheetName val="pow_(final)14"/>
+      <sheetName val="2cl_7x9_modified14"/>
+      <sheetName val="1cl_7x9_Ramon14"/>
+      <sheetName val="1cl_7x7_modified14"/>
+      <sheetName val="2cl_7x7_modified14"/>
+      <sheetName val="1cl_7x9_modified14"/>
+      <sheetName val="3cl_7x9_modified14"/>
+      <sheetName val="2sty4cl_14"/>
+      <sheetName val="2sty6cl_14"/>
+      <sheetName val="2sty8cl_14"/>
+      <sheetName val="h_e_14"/>
+      <sheetName val="cr_attached14"/>
+      <sheetName val="cr_detached14"/>
+      <sheetName val="rc_septic_vault14"/>
+      <sheetName val="chb_septic_vault14"/>
+      <sheetName val="1cl_(2)14"/>
+      <sheetName val="PROGRAM_of_WORK14"/>
+      <sheetName val="1cl_7x7_M14"/>
+      <sheetName val="repair_det_est5"/>
+      <sheetName val="program_of_works5"/>
+      <sheetName val="2cl_7x7_M5"/>
+      <sheetName val="3cl_7x7_M5"/>
+      <sheetName val="1cl_7x9_M5"/>
+      <sheetName val="2cl_7x9_M5"/>
+      <sheetName val="3cl_7x9_M5"/>
+      <sheetName val="4cl_7x9_M5"/>
+      <sheetName val="1cl_7x9_O5"/>
+      <sheetName val="2cl_7x9_O5"/>
+      <sheetName val="2cl_7x9_O_sphere5"/>
+      <sheetName val="3cl_7x9_O5"/>
+      <sheetName val="science_lab5"/>
+      <sheetName val="Typhoon_Resistance_2CL5"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_14"/>
+      <sheetName val="pow_(final)12"/>
+      <sheetName val="2cl_7x9_modified12"/>
+      <sheetName val="1cl_7x9_Ramon12"/>
+      <sheetName val="1cl_7x7_modified12"/>
+      <sheetName val="2cl_7x7_modified12"/>
+      <sheetName val="1cl_7x9_modified12"/>
+      <sheetName val="3cl_7x9_modified12"/>
+      <sheetName val="2sty4cl_12"/>
+      <sheetName val="2sty6cl_12"/>
+      <sheetName val="2sty8cl_12"/>
+      <sheetName val="h_e_12"/>
+      <sheetName val="cr_attached12"/>
+      <sheetName val="cr_detached12"/>
+      <sheetName val="rc_septic_vault12"/>
+      <sheetName val="chb_septic_vault12"/>
+      <sheetName val="1cl_(2)12"/>
+      <sheetName val="PROGRAM_of_WORK12"/>
+      <sheetName val="1cl_7x7_M12"/>
+      <sheetName val="repair_det_est3"/>
+      <sheetName val="program_of_works3"/>
+      <sheetName val="2cl_7x7_M3"/>
+      <sheetName val="3cl_7x7_M3"/>
+      <sheetName val="1cl_7x9_M3"/>
+      <sheetName val="2cl_7x9_M3"/>
+      <sheetName val="3cl_7x9_M3"/>
+      <sheetName val="4cl_7x9_M3"/>
+      <sheetName val="1cl_7x9_O3"/>
+      <sheetName val="2cl_7x9_O3"/>
+      <sheetName val="2cl_7x9_O_sphere3"/>
+      <sheetName val="3cl_7x9_O3"/>
+      <sheetName val="science_lab3"/>
+      <sheetName val="Typhoon_Resistance_2CL3"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_15"/>
+      <sheetName val="pow_(final)13"/>
+      <sheetName val="2cl_7x9_modified13"/>
+      <sheetName val="1cl_7x9_Ramon13"/>
+      <sheetName val="1cl_7x7_modified13"/>
+      <sheetName val="2cl_7x7_modified13"/>
+      <sheetName val="1cl_7x9_modified13"/>
+      <sheetName val="3cl_7x9_modified13"/>
+      <sheetName val="2sty4cl_13"/>
+      <sheetName val="2sty6cl_13"/>
+      <sheetName val="2sty8cl_13"/>
+      <sheetName val="h_e_13"/>
+      <sheetName val="cr_attached13"/>
+      <sheetName val="cr_detached13"/>
+      <sheetName val="rc_septic_vault13"/>
+      <sheetName val="chb_septic_vault13"/>
+      <sheetName val="1cl_(2)13"/>
+      <sheetName val="PROGRAM_of_WORK13"/>
+      <sheetName val="1cl_7x7_M13"/>
+      <sheetName val="repair_det_est4"/>
+      <sheetName val="program_of_works4"/>
+      <sheetName val="2cl_7x7_M4"/>
+      <sheetName val="3cl_7x7_M4"/>
+      <sheetName val="1cl_7x9_M4"/>
+      <sheetName val="2cl_7x9_M4"/>
+      <sheetName val="3cl_7x9_M4"/>
+      <sheetName val="4cl_7x9_M4"/>
+      <sheetName val="1cl_7x9_O4"/>
+      <sheetName val="2cl_7x9_O4"/>
+      <sheetName val="2cl_7x9_O_sphere4"/>
+      <sheetName val="3cl_7x9_O4"/>
+      <sheetName val="science_lab4"/>
+      <sheetName val="Typhoon_Resistance_2CL4"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_17"/>
+      <sheetName val="pow_(final)15"/>
+      <sheetName val="2cl_7x9_modified15"/>
+      <sheetName val="1cl_7x9_Ramon15"/>
+      <sheetName val="1cl_7x7_modified15"/>
+      <sheetName val="2cl_7x7_modified15"/>
+      <sheetName val="1cl_7x9_modified15"/>
+      <sheetName val="3cl_7x9_modified15"/>
+      <sheetName val="2sty4cl_15"/>
+      <sheetName val="2sty6cl_15"/>
+      <sheetName val="2sty8cl_15"/>
+      <sheetName val="h_e_15"/>
+      <sheetName val="cr_attached15"/>
+      <sheetName val="cr_detached15"/>
+      <sheetName val="rc_septic_vault15"/>
+      <sheetName val="chb_septic_vault15"/>
+      <sheetName val="1cl_(2)15"/>
+      <sheetName val="PROGRAM_of_WORK15"/>
+      <sheetName val="1cl_7x7_M15"/>
+      <sheetName val="repair_det_est6"/>
+      <sheetName val="program_of_works6"/>
+      <sheetName val="2cl_7x7_M6"/>
+      <sheetName val="3cl_7x7_M6"/>
+      <sheetName val="1cl_7x9_M6"/>
+      <sheetName val="2cl_7x9_M6"/>
+      <sheetName val="3cl_7x9_M6"/>
+      <sheetName val="4cl_7x9_M6"/>
+      <sheetName val="1cl_7x9_O6"/>
+      <sheetName val="2cl_7x9_O6"/>
+      <sheetName val="2cl_7x9_O_sphere6"/>
+      <sheetName val="3cl_7x9_O6"/>
+      <sheetName val="science_lab6"/>
+      <sheetName val="Typhoon_Resistance_2CL6"/>
+      <sheetName val="DECS_2cl_OMS_(2)5"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)5"/>
+      <sheetName val="DECS_2cl_OMS_(2)3"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)3"/>
+      <sheetName val="DECS_2cl_OMS_(2)1"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)1"/>
+      <sheetName val="DECS_2cl_OMS_(2)2"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)2"/>
+      <sheetName val="DECS_2cl_OMS_(2)4"/>
+      <sheetName val="COP2_okiot_tabuac_bcps(100)4"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_18"/>
+      <sheetName val="pow_(final)16"/>
+      <sheetName val="2cl_7x9_modified16"/>
+      <sheetName val="1cl_7x9_Ramon16"/>
+      <sheetName val="1cl_7x7_modified16"/>
+      <sheetName val="2cl_7x7_modified16"/>
+      <sheetName val="1cl_7x9_modified16"/>
+      <sheetName val="3cl_7x9_modified16"/>
+      <sheetName val="2sty4cl_16"/>
+      <sheetName val="2sty6cl_16"/>
+      <sheetName val="2sty8cl_16"/>
+      <sheetName val="h_e_16"/>
+      <sheetName val="cr_attached16"/>
+      <sheetName val="cr_detached16"/>
+      <sheetName val="rc_septic_vault16"/>
+      <sheetName val="chb_septic_vault16"/>
+      <sheetName val="1cl_(2)16"/>
+      <sheetName val="PROGRAM_of_WORK16"/>
+      <sheetName val="1cl_7x7_M16"/>
+      <sheetName val="repair_det_est7"/>
+      <sheetName val="program_of_works7"/>
+      <sheetName val="2cl_7x7_M7"/>
+      <sheetName val="3cl_7x7_M7"/>
+      <sheetName val="1cl_7x9_M7"/>
+      <sheetName val="2cl_7x9_M7"/>
+      <sheetName val="3cl_7x9_M7"/>
+      <sheetName val="4cl_7x9_M7"/>
+      <sheetName val="1cl_7x9_O7"/>
+      <sheetName val="2cl_7x9_O7"/>
+      <sheetName val="2cl_7x9_O_sphere7"/>
+      <sheetName val="3cl_7x9_O7"/>
+      <sheetName val="science_lab7"/>
+      <sheetName val="Typhoon_Resistance_2CL7"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_20"/>
+      <sheetName val="pow_(final)18"/>
+      <sheetName val="2cl_7x9_modified18"/>
+      <sheetName val="1cl_7x9_Ramon18"/>
+      <sheetName val="1cl_7x7_modified18"/>
+      <sheetName val="2cl_7x7_modified18"/>
+      <sheetName val="1cl_7x9_modified18"/>
+      <sheetName val="3cl_7x9_modified18"/>
+      <sheetName val="2sty4cl_18"/>
+      <sheetName val="2sty6cl_18"/>
+      <sheetName val="2sty8cl_18"/>
+      <sheetName val="h_e_18"/>
+      <sheetName val="cr_attached18"/>
+      <sheetName val="cr_detached18"/>
+      <sheetName val="rc_septic_vault18"/>
+      <sheetName val="chb_septic_vault18"/>
+      <sheetName val="1cl_(2)18"/>
+      <sheetName val="PROGRAM_of_WORK18"/>
+      <sheetName val="1cl_7x7_M18"/>
+      <sheetName val="repair_det_est9"/>
+      <sheetName val="program_of_works9"/>
+      <sheetName val="2cl_7x7_M9"/>
+      <sheetName val="3cl_7x7_M9"/>
+      <sheetName val="1cl_7x9_M9"/>
+      <sheetName val="2cl_7x9_M9"/>
+      <sheetName val="3cl_7x9_M9"/>
+      <sheetName val="4cl_7x9_M9"/>
+      <sheetName val="1cl_7x9_O9"/>
+      <sheetName val="2cl_7x9_O9"/>
+      <sheetName val="2cl_7x9_O_sphere9"/>
+      <sheetName val="3cl_7x9_O9"/>
+      <sheetName val="science_lab9"/>
+      <sheetName val="Typhoon_Resistance_2CL9"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_22"/>
+      <sheetName val="pow_(final)20"/>
+      <sheetName val="2cl_7x9_modified20"/>
+      <sheetName val="1cl_7x9_Ramon20"/>
+      <sheetName val="1cl_7x7_modified20"/>
+      <sheetName val="2cl_7x7_modified20"/>
+      <sheetName val="1cl_7x9_modified20"/>
+      <sheetName val="3cl_7x9_modified20"/>
+      <sheetName val="2sty4cl_20"/>
+      <sheetName val="2sty6cl_20"/>
+      <sheetName val="2sty8cl_20"/>
+      <sheetName val="h_e_20"/>
+      <sheetName val="cr_attached20"/>
+      <sheetName val="cr_detached20"/>
+      <sheetName val="rc_septic_vault20"/>
+      <sheetName val="chb_septic_vault20"/>
+      <sheetName val="1cl_(2)20"/>
+      <sheetName val="PROGRAM_of_WORK20"/>
+      <sheetName val="1cl_7x7_M20"/>
+      <sheetName val="repair_det_est11"/>
+      <sheetName val="program_of_works11"/>
+      <sheetName val="2cl_7x7_M11"/>
+      <sheetName val="3cl_7x7_M11"/>
+      <sheetName val="1cl_7x9_M11"/>
+      <sheetName val="2cl_7x9_M11"/>
+      <sheetName val="3cl_7x9_M11"/>
+      <sheetName val="4cl_7x9_M11"/>
+      <sheetName val="1cl_7x9_O11"/>
+      <sheetName val="2cl_7x9_O11"/>
+      <sheetName val="2cl_7x9_O_sphere11"/>
+      <sheetName val="3cl_7x9_O11"/>
+      <sheetName val="science_lab11"/>
+      <sheetName val="Typhoon_Resistance_2CL11"/>
+      <sheetName val="1cl_7x9_modified_wo_ceiling_21"/>
+      <sheetName val="pow_(final)19"/>
+      <sheetName val="2cl_7x9_modified19"/>
+      <sheetName val="1cl_7x9_Ramon19"/>
+      <sheetName val="1cl_7x7_modified19"/>
+      <sheetName val="2cl_7x7_modified19"/>
+      <sheetName val="1cl_7x9_modified19"/>
+      <sheetName val="3cl_7x9_modified19"/>
+      <sheetName val="2sty4cl_19"/>
+      <sheetName val="2sty6cl_19"/>
+      <sheetName val="2sty8cl_19"/>
+      <sheetName val="h_e_19"/>
+      <sheetName val="cr_attached19"/>
+      <sheetName val="cr_detached19"/>
+      <sheetName val="rc_septic_vault19"/>
+      <sheetName val="chb_septic_vault19"/>
+      <sheetName val="1cl_(2)19"/>
+      <sheetName val="PROGRAM_of_WORK19"/>
+      <sheetName val="1cl_7x7_M19"/>
+      <sheetName val="repair_det_est10"/>
+      <sheetName val="program_of_works10"/>
+      <sheetName val="2cl_7x7_M10"/>
+      <sheetName val="3cl_7x7_M10"/>
+      <sheetName val="1cl_7x9_M10"/>
+      <sheetName val="2cl_7x9_M10"/>
+      <sheetName val="3cl_7x9_M10"/>
+      <sheetName val="4cl_7x9_M10"/>
+      <sheetName val="1cl_7x9_O10"/>
+      <sheetName val="2cl_7x9_O10"/>
+      <sheetName val="2cl_7x9_O_sphere10"/>
+      <sheetName val="3cl_7x9_O10"/>
+      <sheetName val="science_lab10"/>
+      <sheetName val="Typhoon_Resistance_2CL10"/>
+      <sheetName val="Detailed_Estimate1"/>
+      <sheetName val="unit_weight_of_angle_bars1"/>
+      <sheetName val="unit_weight_of_purlins1"/>
+      <sheetName val="NEWCON_2017_(CL)1"/>
+      <sheetName val="BEFF_20161"/>
+      <sheetName val="Account_Type1"/>
+      <sheetName val="Source_of_data"/>
+      <sheetName val="⋜ú曆衟Ùꩋᄷ}衭_x0009_d駒ÿ꫏ì蠱"/>
+      <sheetName val="Costs and Types"/>
+      <sheetName val="GRAND SUM"/>
+      <sheetName val="Summary Conf Rm"/>
+      <sheetName val="DET CONF RM"/>
+      <sheetName val="rc ceptic vault"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
+      <sheetData sheetId="34"/>
+      <sheetData sheetId="35"/>
+      <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
+      <sheetData sheetId="38"/>
+      <sheetData sheetId="39"/>
+      <sheetData sheetId="40"/>
+      <sheetData sheetId="41"/>
+      <sheetData sheetId="42"/>
+      <sheetData sheetId="43"/>
+      <sheetData sheetId="44"/>
+      <sheetData sheetId="45"/>
+      <sheetData sheetId="46"/>
+      <sheetData sheetId="47"/>
+      <sheetData sheetId="48"/>
+      <sheetData sheetId="49"/>
+      <sheetData sheetId="50"/>
+      <sheetData sheetId="51"/>
+      <sheetData sheetId="52"/>
+      <sheetData sheetId="53"/>
+      <sheetData sheetId="54"/>
+      <sheetData sheetId="55"/>
+      <sheetData sheetId="56"/>
+      <sheetData sheetId="57"/>
+      <sheetData sheetId="58"/>
+      <sheetData sheetId="59"/>
+      <sheetData sheetId="60"/>
+      <sheetData sheetId="61"/>
+      <sheetData sheetId="62"/>
+      <sheetData sheetId="63"/>
+      <sheetData sheetId="64"/>
+      <sheetData sheetId="65"/>
+      <sheetData sheetId="66"/>
+      <sheetData sheetId="67"/>
+      <sheetData sheetId="68"/>
+      <sheetData sheetId="69"/>
+      <sheetData sheetId="70"/>
+      <sheetData sheetId="71"/>
+      <sheetData sheetId="72"/>
+      <sheetData sheetId="73"/>
+      <sheetData sheetId="74"/>
+      <sheetData sheetId="75"/>
+      <sheetData sheetId="76"/>
+      <sheetData sheetId="77"/>
+      <sheetData sheetId="78"/>
+      <sheetData sheetId="79"/>
+      <sheetData sheetId="80"/>
+      <sheetData sheetId="81"/>
+      <sheetData sheetId="82"/>
+      <sheetData sheetId="83"/>
+      <sheetData sheetId="84"/>
+      <sheetData sheetId="85"/>
+      <sheetData sheetId="86"/>
+      <sheetData sheetId="87"/>
+      <sheetData sheetId="88"/>
+      <sheetData sheetId="89"/>
+      <sheetData sheetId="90"/>
+      <sheetData sheetId="91"/>
+      <sheetData sheetId="92"/>
+      <sheetData sheetId="93"/>
+      <sheetData sheetId="94"/>
+      <sheetData sheetId="95"/>
+      <sheetData sheetId="96"/>
+      <sheetData sheetId="97"/>
+      <sheetData sheetId="98"/>
+      <sheetData sheetId="99"/>
+      <sheetData sheetId="100"/>
+      <sheetData sheetId="101"/>
+      <sheetData sheetId="102"/>
+      <sheetData sheetId="103"/>
+      <sheetData sheetId="104"/>
+      <sheetData sheetId="105"/>
+      <sheetData sheetId="106"/>
+      <sheetData sheetId="107"/>
+      <sheetData sheetId="108"/>
+      <sheetData sheetId="109"/>
+      <sheetData sheetId="110"/>
+      <sheetData sheetId="111"/>
+      <sheetData sheetId="112"/>
+      <sheetData sheetId="113"/>
+      <sheetData sheetId="114"/>
+      <sheetData sheetId="115"/>
+      <sheetData sheetId="116"/>
+      <sheetData sheetId="117"/>
+      <sheetData sheetId="118"/>
+      <sheetData sheetId="119"/>
+      <sheetData sheetId="120"/>
+      <sheetData sheetId="121"/>
+      <sheetData sheetId="122"/>
+      <sheetData sheetId="123"/>
+      <sheetData sheetId="124"/>
+      <sheetData sheetId="125"/>
+      <sheetData sheetId="126"/>
+      <sheetData sheetId="127"/>
+      <sheetData sheetId="128"/>
+      <sheetData sheetId="129"/>
+      <sheetData sheetId="130"/>
+      <sheetData sheetId="131"/>
+      <sheetData sheetId="132"/>
+      <sheetData sheetId="133"/>
+      <sheetData sheetId="134"/>
+      <sheetData sheetId="135"/>
+      <sheetData sheetId="136"/>
+      <sheetData sheetId="137"/>
+      <sheetData sheetId="138"/>
+      <sheetData sheetId="139"/>
+      <sheetData sheetId="140"/>
+      <sheetData sheetId="141"/>
+      <sheetData sheetId="142"/>
+      <sheetData sheetId="143"/>
+      <sheetData sheetId="144"/>
+      <sheetData sheetId="145"/>
+      <sheetData sheetId="146"/>
+      <sheetData sheetId="147"/>
+      <sheetData sheetId="148"/>
+      <sheetData sheetId="149"/>
+      <sheetData sheetId="150"/>
+      <sheetData sheetId="151"/>
+      <sheetData sheetId="152"/>
+      <sheetData sheetId="153"/>
+      <sheetData sheetId="154"/>
+      <sheetData sheetId="155"/>
+      <sheetData sheetId="156"/>
+      <sheetData sheetId="157"/>
+      <sheetData sheetId="158"/>
+      <sheetData sheetId="159"/>
+      <sheetData sheetId="160"/>
+      <sheetData sheetId="161"/>
+      <sheetData sheetId="162"/>
+      <sheetData sheetId="163"/>
+      <sheetData sheetId="164"/>
+      <sheetData sheetId="165"/>
+      <sheetData sheetId="166"/>
+      <sheetData sheetId="167"/>
+      <sheetData sheetId="168"/>
+      <sheetData sheetId="169"/>
+      <sheetData sheetId="170"/>
+      <sheetData sheetId="171"/>
+      <sheetData sheetId="172"/>
+      <sheetData sheetId="173"/>
+      <sheetData sheetId="174"/>
+      <sheetData sheetId="175"/>
+      <sheetData sheetId="176"/>
+      <sheetData sheetId="177"/>
+      <sheetData sheetId="178"/>
+      <sheetData sheetId="179"/>
+      <sheetData sheetId="180"/>
+      <sheetData sheetId="181"/>
+      <sheetData sheetId="182"/>
+      <sheetData sheetId="183"/>
+      <sheetData sheetId="184"/>
+      <sheetData sheetId="185"/>
+      <sheetData sheetId="186"/>
+      <sheetData sheetId="187"/>
+      <sheetData sheetId="188"/>
+      <sheetData sheetId="189"/>
+      <sheetData sheetId="190"/>
+      <sheetData sheetId="191"/>
+      <sheetData sheetId="192"/>
+      <sheetData sheetId="193"/>
+      <sheetData sheetId="194"/>
+      <sheetData sheetId="195"/>
+      <sheetData sheetId="196"/>
+      <sheetData sheetId="197"/>
+      <sheetData sheetId="198"/>
+      <sheetData sheetId="199"/>
+      <sheetData sheetId="200"/>
+      <sheetData sheetId="201"/>
+      <sheetData sheetId="202"/>
+      <sheetData sheetId="203"/>
+      <sheetData sheetId="204"/>
+      <sheetData sheetId="205"/>
+      <sheetData sheetId="206"/>
+      <sheetData sheetId="207"/>
+      <sheetData sheetId="208" refreshError="1"/>
+      <sheetData sheetId="209"/>
+      <sheetData sheetId="210"/>
+      <sheetData sheetId="211"/>
+      <sheetData sheetId="212"/>
+      <sheetData sheetId="213"/>
+      <sheetData sheetId="214"/>
+      <sheetData sheetId="215"/>
+      <sheetData sheetId="216"/>
+      <sheetData sheetId="217"/>
+      <sheetData sheetId="218"/>
+      <sheetData sheetId="219"/>
+      <sheetData sheetId="220"/>
+      <sheetData sheetId="221"/>
+      <sheetData sheetId="222"/>
+      <sheetData sheetId="223"/>
+      <sheetData sheetId="224"/>
+      <sheetData sheetId="225"/>
+      <sheetData sheetId="226"/>
+      <sheetData sheetId="227"/>
+      <sheetData sheetId="228"/>
+      <sheetData sheetId="229"/>
+      <sheetData sheetId="230"/>
+      <sheetData sheetId="231"/>
+      <sheetData sheetId="232"/>
+      <sheetData sheetId="233"/>
+      <sheetData sheetId="234"/>
+      <sheetData sheetId="235"/>
+      <sheetData sheetId="236"/>
+      <sheetData sheetId="237"/>
+      <sheetData sheetId="238"/>
+      <sheetData sheetId="239" refreshError="1"/>
+      <sheetData sheetId="240" refreshError="1"/>
+      <sheetData sheetId="241" refreshError="1"/>
+      <sheetData sheetId="242"/>
+      <sheetData sheetId="243"/>
+      <sheetData sheetId="244" refreshError="1"/>
+      <sheetData sheetId="245"/>
+      <sheetData sheetId="246"/>
+      <sheetData sheetId="247"/>
+      <sheetData sheetId="248"/>
+      <sheetData sheetId="249"/>
+      <sheetData sheetId="250"/>
+      <sheetData sheetId="251"/>
+      <sheetData sheetId="252"/>
+      <sheetData sheetId="253"/>
+      <sheetData sheetId="254"/>
+      <sheetData sheetId="255"/>
+      <sheetData sheetId="256" refreshError="1"/>
+      <sheetData sheetId="257" refreshError="1"/>
+      <sheetData sheetId="258" refreshError="1"/>
+      <sheetData sheetId="259" refreshError="1"/>
+      <sheetData sheetId="260" refreshError="1"/>
+      <sheetData sheetId="261" refreshError="1"/>
+      <sheetData sheetId="262" refreshError="1"/>
+      <sheetData sheetId="263" refreshError="1"/>
+      <sheetData sheetId="264" refreshError="1"/>
+      <sheetData sheetId="265" refreshError="1"/>
+      <sheetData sheetId="266" refreshError="1"/>
+      <sheetData sheetId="267" refreshError="1"/>
+      <sheetData sheetId="268" refreshError="1"/>
+      <sheetData sheetId="269" refreshError="1"/>
+      <sheetData sheetId="270" refreshError="1"/>
+      <sheetData sheetId="271" refreshError="1"/>
+      <sheetData sheetId="272" refreshError="1"/>
+      <sheetData sheetId="273" refreshError="1"/>
+      <sheetData sheetId="274" refreshError="1"/>
+      <sheetData sheetId="275" refreshError="1"/>
+      <sheetData sheetId="276" refreshError="1"/>
+      <sheetData sheetId="277" refreshError="1"/>
+      <sheetData sheetId="278" refreshError="1"/>
+      <sheetData sheetId="279" refreshError="1"/>
+      <sheetData sheetId="280" refreshError="1"/>
+      <sheetData sheetId="281" refreshError="1"/>
+      <sheetData sheetId="282" refreshError="1"/>
+      <sheetData sheetId="283" refreshError="1"/>
+      <sheetData sheetId="284" refreshError="1"/>
+      <sheetData sheetId="285" refreshError="1"/>
+      <sheetData sheetId="286" refreshError="1"/>
+      <sheetData sheetId="287" refreshError="1"/>
+      <sheetData sheetId="288" refreshError="1"/>
+      <sheetData sheetId="289" refreshError="1"/>
+      <sheetData sheetId="290" refreshError="1"/>
+      <sheetData sheetId="291" refreshError="1"/>
+      <sheetData sheetId="292" refreshError="1"/>
+      <sheetData sheetId="293" refreshError="1"/>
+      <sheetData sheetId="294" refreshError="1"/>
+      <sheetData sheetId="295" refreshError="1"/>
+      <sheetData sheetId="296" refreshError="1"/>
+      <sheetData sheetId="297" refreshError="1"/>
+      <sheetData sheetId="298" refreshError="1"/>
+      <sheetData sheetId="299" refreshError="1"/>
+      <sheetData sheetId="300" refreshError="1"/>
+      <sheetData sheetId="301" refreshError="1"/>
+      <sheetData sheetId="302" refreshError="1"/>
+      <sheetData sheetId="303" refreshError="1"/>
+      <sheetData sheetId="304" refreshError="1"/>
+      <sheetData sheetId="305" refreshError="1"/>
+      <sheetData sheetId="306" refreshError="1"/>
+      <sheetData sheetId="307" refreshError="1"/>
+      <sheetData sheetId="308" refreshError="1"/>
+      <sheetData sheetId="309" refreshError="1"/>
+      <sheetData sheetId="310" refreshError="1"/>
+      <sheetData sheetId="311" refreshError="1"/>
+      <sheetData sheetId="312" refreshError="1"/>
+      <sheetData sheetId="313" refreshError="1"/>
+      <sheetData sheetId="314" refreshError="1"/>
+      <sheetData sheetId="315" refreshError="1"/>
+      <sheetData sheetId="316" refreshError="1"/>
+      <sheetData sheetId="317" refreshError="1"/>
+      <sheetData sheetId="318" refreshError="1"/>
+      <sheetData sheetId="319" refreshError="1"/>
+      <sheetData sheetId="320" refreshError="1"/>
+      <sheetData sheetId="321" refreshError="1"/>
+      <sheetData sheetId="322" refreshError="1"/>
+      <sheetData sheetId="323" refreshError="1"/>
+      <sheetData sheetId="324" refreshError="1"/>
+      <sheetData sheetId="325" refreshError="1"/>
+      <sheetData sheetId="326" refreshError="1"/>
+      <sheetData sheetId="327" refreshError="1"/>
+      <sheetData sheetId="328" refreshError="1"/>
+      <sheetData sheetId="329" refreshError="1"/>
+      <sheetData sheetId="330" refreshError="1"/>
+      <sheetData sheetId="331" refreshError="1"/>
+      <sheetData sheetId="332" refreshError="1"/>
+      <sheetData sheetId="333" refreshError="1"/>
+      <sheetData sheetId="334" refreshError="1"/>
+      <sheetData sheetId="335" refreshError="1"/>
+      <sheetData sheetId="336" refreshError="1"/>
+      <sheetData sheetId="337" refreshError="1"/>
+      <sheetData sheetId="338" refreshError="1"/>
+      <sheetData sheetId="339" refreshError="1"/>
+      <sheetData sheetId="340" refreshError="1"/>
+      <sheetData sheetId="341" refreshError="1"/>
+      <sheetData sheetId="342" refreshError="1"/>
+      <sheetData sheetId="343" refreshError="1"/>
+      <sheetData sheetId="344" refreshError="1"/>
+      <sheetData sheetId="345" refreshError="1"/>
+      <sheetData sheetId="346" refreshError="1"/>
+      <sheetData sheetId="347" refreshError="1"/>
+      <sheetData sheetId="348" refreshError="1"/>
+      <sheetData sheetId="349" refreshError="1"/>
+      <sheetData sheetId="350" refreshError="1"/>
+      <sheetData sheetId="351" refreshError="1"/>
+      <sheetData sheetId="352" refreshError="1"/>
+      <sheetData sheetId="353" refreshError="1"/>
+      <sheetData sheetId="354" refreshError="1"/>
+      <sheetData sheetId="355" refreshError="1"/>
+      <sheetData sheetId="356" refreshError="1"/>
+      <sheetData sheetId="357" refreshError="1"/>
+      <sheetData sheetId="358" refreshError="1"/>
+      <sheetData sheetId="359" refreshError="1"/>
+      <sheetData sheetId="360" refreshError="1"/>
+      <sheetData sheetId="361" refreshError="1"/>
+      <sheetData sheetId="362" refreshError="1"/>
+      <sheetData sheetId="363" refreshError="1"/>
+      <sheetData sheetId="364" refreshError="1"/>
+      <sheetData sheetId="365" refreshError="1"/>
+      <sheetData sheetId="366" refreshError="1"/>
+      <sheetData sheetId="367" refreshError="1"/>
+      <sheetData sheetId="368" refreshError="1"/>
+      <sheetData sheetId="369" refreshError="1"/>
+      <sheetData sheetId="370" refreshError="1"/>
+      <sheetData sheetId="371" refreshError="1"/>
+      <sheetData sheetId="372" refreshError="1"/>
+      <sheetData sheetId="373" refreshError="1"/>
+      <sheetData sheetId="374" refreshError="1"/>
+      <sheetData sheetId="375" refreshError="1"/>
+      <sheetData sheetId="376" refreshError="1"/>
+      <sheetData sheetId="377" refreshError="1"/>
+      <sheetData sheetId="378" refreshError="1"/>
+      <sheetData sheetId="379" refreshError="1"/>
+      <sheetData sheetId="380" refreshError="1"/>
+      <sheetData sheetId="381" refreshError="1"/>
+      <sheetData sheetId="382" refreshError="1"/>
+      <sheetData sheetId="383" refreshError="1"/>
+      <sheetData sheetId="384" refreshError="1"/>
+      <sheetData sheetId="385" refreshError="1"/>
+      <sheetData sheetId="386" refreshError="1"/>
+      <sheetData sheetId="387" refreshError="1"/>
+      <sheetData sheetId="388" refreshError="1"/>
+      <sheetData sheetId="389" refreshError="1"/>
+      <sheetData sheetId="390" refreshError="1"/>
+      <sheetData sheetId="391" refreshError="1"/>
+      <sheetData sheetId="392" refreshError="1"/>
+      <sheetData sheetId="393" refreshError="1"/>
+      <sheetData sheetId="394" refreshError="1"/>
+      <sheetData sheetId="395" refreshError="1"/>
+      <sheetData sheetId="396" refreshError="1"/>
+      <sheetData sheetId="397" refreshError="1"/>
+      <sheetData sheetId="398" refreshError="1"/>
+      <sheetData sheetId="399" refreshError="1"/>
+      <sheetData sheetId="400" refreshError="1"/>
+      <sheetData sheetId="401" refreshError="1"/>
+      <sheetData sheetId="402" refreshError="1"/>
+      <sheetData sheetId="403" refreshError="1"/>
+      <sheetData sheetId="404" refreshError="1"/>
+      <sheetData sheetId="405" refreshError="1"/>
+      <sheetData sheetId="406" refreshError="1"/>
+      <sheetData sheetId="407" refreshError="1"/>
+      <sheetData sheetId="408" refreshError="1"/>
+      <sheetData sheetId="409" refreshError="1"/>
+      <sheetData sheetId="410" refreshError="1"/>
+      <sheetData sheetId="411" refreshError="1"/>
+      <sheetData sheetId="412" refreshError="1"/>
+      <sheetData sheetId="413" refreshError="1"/>
+      <sheetData sheetId="414" refreshError="1"/>
+      <sheetData sheetId="415" refreshError="1"/>
+      <sheetData sheetId="416" refreshError="1"/>
+      <sheetData sheetId="417" refreshError="1"/>
+      <sheetData sheetId="418" refreshError="1"/>
+      <sheetData sheetId="419" refreshError="1"/>
+      <sheetData sheetId="420" refreshError="1"/>
+      <sheetData sheetId="421" refreshError="1"/>
+      <sheetData sheetId="422" refreshError="1"/>
+      <sheetData sheetId="423" refreshError="1"/>
+      <sheetData sheetId="424" refreshError="1"/>
+      <sheetData sheetId="425" refreshError="1"/>
+      <sheetData sheetId="426" refreshError="1"/>
+      <sheetData sheetId="427" refreshError="1"/>
+      <sheetData sheetId="428" refreshError="1"/>
+      <sheetData sheetId="429" refreshError="1"/>
+      <sheetData sheetId="430" refreshError="1"/>
+      <sheetData sheetId="431"/>
+      <sheetData sheetId="432"/>
+      <sheetData sheetId="433"/>
+      <sheetData sheetId="434"/>
+      <sheetData sheetId="435"/>
+      <sheetData sheetId="436"/>
+      <sheetData sheetId="437"/>
+      <sheetData sheetId="438"/>
+      <sheetData sheetId="439"/>
+      <sheetData sheetId="440"/>
+      <sheetData sheetId="441"/>
+      <sheetData sheetId="442"/>
+      <sheetData sheetId="443"/>
+      <sheetData sheetId="444"/>
+      <sheetData sheetId="445"/>
+      <sheetData sheetId="446"/>
+      <sheetData sheetId="447"/>
+      <sheetData sheetId="448"/>
+      <sheetData sheetId="449"/>
+      <sheetData sheetId="450"/>
+      <sheetData sheetId="451"/>
+      <sheetData sheetId="452"/>
+      <sheetData sheetId="453"/>
+      <sheetData sheetId="454"/>
+      <sheetData sheetId="455"/>
+      <sheetData sheetId="456"/>
+      <sheetData sheetId="457"/>
+      <sheetData sheetId="458"/>
+      <sheetData sheetId="459"/>
+      <sheetData sheetId="460"/>
+      <sheetData sheetId="461"/>
+      <sheetData sheetId="462"/>
+      <sheetData sheetId="463"/>
+      <sheetData sheetId="464"/>
+      <sheetData sheetId="465"/>
+      <sheetData sheetId="466"/>
+      <sheetData sheetId="467"/>
+      <sheetData sheetId="468"/>
+      <sheetData sheetId="469"/>
+      <sheetData sheetId="470"/>
+      <sheetData sheetId="471"/>
+      <sheetData sheetId="472"/>
+      <sheetData sheetId="473"/>
+      <sheetData sheetId="474"/>
+      <sheetData sheetId="475"/>
+      <sheetData sheetId="476"/>
+      <sheetData sheetId="477"/>
+      <sheetData sheetId="478"/>
+      <sheetData sheetId="479"/>
+      <sheetData sheetId="480"/>
+      <sheetData sheetId="481"/>
+      <sheetData sheetId="482"/>
+      <sheetData sheetId="483"/>
+      <sheetData sheetId="484"/>
+      <sheetData sheetId="485"/>
+      <sheetData sheetId="486"/>
+      <sheetData sheetId="487"/>
+      <sheetData sheetId="488"/>
+      <sheetData sheetId="489"/>
+      <sheetData sheetId="490"/>
+      <sheetData sheetId="491"/>
+      <sheetData sheetId="492"/>
+      <sheetData sheetId="493"/>
+      <sheetData sheetId="494"/>
+      <sheetData sheetId="495"/>
+      <sheetData sheetId="496"/>
+      <sheetData sheetId="497"/>
+      <sheetData sheetId="498"/>
+      <sheetData sheetId="499"/>
+      <sheetData sheetId="500"/>
+      <sheetData sheetId="501"/>
+      <sheetData sheetId="502"/>
+      <sheetData sheetId="503"/>
+      <sheetData sheetId="504"/>
+      <sheetData sheetId="505"/>
+      <sheetData sheetId="506"/>
+      <sheetData sheetId="507"/>
+      <sheetData sheetId="508"/>
+      <sheetData sheetId="509"/>
+      <sheetData sheetId="510"/>
+      <sheetData sheetId="511"/>
+      <sheetData sheetId="512"/>
+      <sheetData sheetId="513"/>
+      <sheetData sheetId="514"/>
+      <sheetData sheetId="515"/>
+      <sheetData sheetId="516"/>
+      <sheetData sheetId="517"/>
+      <sheetData sheetId="518"/>
+      <sheetData sheetId="519"/>
+      <sheetData sheetId="520"/>
+      <sheetData sheetId="521"/>
+      <sheetData sheetId="522"/>
+      <sheetData sheetId="523"/>
+      <sheetData sheetId="524"/>
+      <sheetData sheetId="525"/>
+      <sheetData sheetId="526"/>
+      <sheetData sheetId="527"/>
+      <sheetData sheetId="528"/>
+      <sheetData sheetId="529"/>
+      <sheetData sheetId="530"/>
+      <sheetData sheetId="531"/>
+      <sheetData sheetId="532"/>
+      <sheetData sheetId="533"/>
+      <sheetData sheetId="534"/>
+      <sheetData sheetId="535"/>
+      <sheetData sheetId="536"/>
+      <sheetData sheetId="537"/>
+      <sheetData sheetId="538"/>
+      <sheetData sheetId="539"/>
+      <sheetData sheetId="540"/>
+      <sheetData sheetId="541"/>
+      <sheetData sheetId="542"/>
+      <sheetData sheetId="543"/>
+      <sheetData sheetId="544"/>
+      <sheetData sheetId="545"/>
+      <sheetData sheetId="546"/>
+      <sheetData sheetId="547"/>
+      <sheetData sheetId="548"/>
+      <sheetData sheetId="549"/>
+      <sheetData sheetId="550"/>
+      <sheetData sheetId="551"/>
+      <sheetData sheetId="552"/>
+      <sheetData sheetId="553"/>
+      <sheetData sheetId="554"/>
+      <sheetData sheetId="555"/>
+      <sheetData sheetId="556"/>
+      <sheetData sheetId="557"/>
+      <sheetData sheetId="558"/>
+      <sheetData sheetId="559"/>
+      <sheetData sheetId="560"/>
+      <sheetData sheetId="561"/>
+      <sheetData sheetId="562"/>
+      <sheetData sheetId="563"/>
+      <sheetData sheetId="564"/>
+      <sheetData sheetId="565"/>
+      <sheetData sheetId="566"/>
+      <sheetData sheetId="567"/>
+      <sheetData sheetId="568"/>
+      <sheetData sheetId="569"/>
+      <sheetData sheetId="570"/>
+      <sheetData sheetId="571"/>
+      <sheetData sheetId="572"/>
+      <sheetData sheetId="573"/>
+      <sheetData sheetId="574"/>
+      <sheetData sheetId="575"/>
+      <sheetData sheetId="576"/>
+      <sheetData sheetId="577"/>
+      <sheetData sheetId="578"/>
+      <sheetData sheetId="579"/>
+      <sheetData sheetId="580"/>
+      <sheetData sheetId="581"/>
+      <sheetData sheetId="582"/>
+      <sheetData sheetId="583"/>
+      <sheetData sheetId="584"/>
+      <sheetData sheetId="585"/>
+      <sheetData sheetId="586"/>
+      <sheetData sheetId="587"/>
+      <sheetData sheetId="588"/>
+      <sheetData sheetId="589"/>
+      <sheetData sheetId="590"/>
+      <sheetData sheetId="591"/>
+      <sheetData sheetId="592"/>
+      <sheetData sheetId="593"/>
+      <sheetData sheetId="594"/>
+      <sheetData sheetId="595"/>
+      <sheetData sheetId="596"/>
+      <sheetData sheetId="597"/>
+      <sheetData sheetId="598"/>
+      <sheetData sheetId="599"/>
+      <sheetData sheetId="600"/>
+      <sheetData sheetId="601"/>
+      <sheetData sheetId="602"/>
+      <sheetData sheetId="603"/>
+      <sheetData sheetId="604"/>
+      <sheetData sheetId="605"/>
+      <sheetData sheetId="606"/>
+      <sheetData sheetId="607"/>
+      <sheetData sheetId="608"/>
+      <sheetData sheetId="609"/>
+      <sheetData sheetId="610"/>
+      <sheetData sheetId="611"/>
+      <sheetData sheetId="612"/>
+      <sheetData sheetId="613"/>
+      <sheetData sheetId="614"/>
+      <sheetData sheetId="615"/>
+      <sheetData sheetId="616"/>
+      <sheetData sheetId="617"/>
+      <sheetData sheetId="618"/>
+      <sheetData sheetId="619"/>
+      <sheetData sheetId="620"/>
+      <sheetData sheetId="621"/>
+      <sheetData sheetId="622"/>
+      <sheetData sheetId="623"/>
+      <sheetData sheetId="624"/>
+      <sheetData sheetId="625"/>
+      <sheetData sheetId="626"/>
+      <sheetData sheetId="627"/>
+      <sheetData sheetId="628"/>
+      <sheetData sheetId="629"/>
+      <sheetData sheetId="630"/>
+      <sheetData sheetId="631"/>
+      <sheetData sheetId="632"/>
+      <sheetData sheetId="633"/>
+      <sheetData sheetId="634"/>
+      <sheetData sheetId="635"/>
+      <sheetData sheetId="636"/>
+      <sheetData sheetId="637"/>
+      <sheetData sheetId="638"/>
+      <sheetData sheetId="639"/>
+      <sheetData sheetId="640"/>
+      <sheetData sheetId="641"/>
+      <sheetData sheetId="642"/>
+      <sheetData sheetId="643"/>
+      <sheetData sheetId="644"/>
+      <sheetData sheetId="645"/>
+      <sheetData sheetId="646"/>
+      <sheetData sheetId="647"/>
+      <sheetData sheetId="648"/>
+      <sheetData sheetId="649"/>
+      <sheetData sheetId="650"/>
+      <sheetData sheetId="651"/>
+      <sheetData sheetId="652"/>
+      <sheetData sheetId="653"/>
+      <sheetData sheetId="654"/>
+      <sheetData sheetId="655"/>
+      <sheetData sheetId="656"/>
+      <sheetData sheetId="657"/>
+      <sheetData sheetId="658"/>
+      <sheetData sheetId="659"/>
+      <sheetData sheetId="660"/>
+      <sheetData sheetId="661"/>
+      <sheetData sheetId="662"/>
+      <sheetData sheetId="663"/>
+      <sheetData sheetId="664"/>
+      <sheetData sheetId="665"/>
+      <sheetData sheetId="666"/>
+      <sheetData sheetId="667"/>
+      <sheetData sheetId="668"/>
+      <sheetData sheetId="669"/>
+      <sheetData sheetId="670"/>
+      <sheetData sheetId="671"/>
+      <sheetData sheetId="672"/>
+      <sheetData sheetId="673"/>
+      <sheetData sheetId="674"/>
+      <sheetData sheetId="675"/>
+      <sheetData sheetId="676"/>
+      <sheetData sheetId="677"/>
+      <sheetData sheetId="678"/>
+      <sheetData sheetId="679"/>
+      <sheetData sheetId="680"/>
+      <sheetData sheetId="681"/>
+      <sheetData sheetId="682"/>
+      <sheetData sheetId="683"/>
+      <sheetData sheetId="684"/>
+      <sheetData sheetId="685"/>
+      <sheetData sheetId="686"/>
+      <sheetData sheetId="687"/>
+      <sheetData sheetId="688"/>
+      <sheetData sheetId="689"/>
+      <sheetData sheetId="690"/>
+      <sheetData sheetId="691"/>
+      <sheetData sheetId="692"/>
+      <sheetData sheetId="693"/>
+      <sheetData sheetId="694"/>
+      <sheetData sheetId="695"/>
+      <sheetData sheetId="696"/>
+      <sheetData sheetId="697"/>
+      <sheetData sheetId="698"/>
+      <sheetData sheetId="699"/>
+      <sheetData sheetId="700"/>
+      <sheetData sheetId="701"/>
+      <sheetData sheetId="702"/>
+      <sheetData sheetId="703"/>
+      <sheetData sheetId="704"/>
+      <sheetData sheetId="705"/>
+      <sheetData sheetId="706"/>
+      <sheetData sheetId="707"/>
+      <sheetData sheetId="708"/>
+      <sheetData sheetId="709"/>
+      <sheetData sheetId="710"/>
+      <sheetData sheetId="711"/>
+      <sheetData sheetId="712"/>
+      <sheetData sheetId="713"/>
+      <sheetData sheetId="714"/>
+      <sheetData sheetId="715"/>
+      <sheetData sheetId="716"/>
+      <sheetData sheetId="717"/>
+      <sheetData sheetId="718"/>
+      <sheetData sheetId="719"/>
+      <sheetData sheetId="720"/>
+      <sheetData sheetId="721"/>
+      <sheetData sheetId="722"/>
+      <sheetData sheetId="723"/>
+      <sheetData sheetId="724"/>
+      <sheetData sheetId="725"/>
+      <sheetData sheetId="726"/>
+      <sheetData sheetId="727"/>
+      <sheetData sheetId="728"/>
+      <sheetData sheetId="729"/>
+      <sheetData sheetId="730"/>
+      <sheetData sheetId="731"/>
+      <sheetData sheetId="732"/>
+      <sheetData sheetId="733"/>
+      <sheetData sheetId="734"/>
+      <sheetData sheetId="735"/>
+      <sheetData sheetId="736"/>
+      <sheetData sheetId="737"/>
+      <sheetData sheetId="738"/>
+      <sheetData sheetId="739"/>
+      <sheetData sheetId="740"/>
+      <sheetData sheetId="741"/>
+      <sheetData sheetId="742"/>
+      <sheetData sheetId="743"/>
+      <sheetData sheetId="744"/>
+      <sheetData sheetId="745"/>
+      <sheetData sheetId="746"/>
+      <sheetData sheetId="747"/>
+      <sheetData sheetId="748"/>
+      <sheetData sheetId="749"/>
+      <sheetData sheetId="750"/>
+      <sheetData sheetId="751"/>
+      <sheetData sheetId="752"/>
+      <sheetData sheetId="753"/>
+      <sheetData sheetId="754"/>
+      <sheetData sheetId="755"/>
+      <sheetData sheetId="756"/>
+      <sheetData sheetId="757"/>
+      <sheetData sheetId="758"/>
+      <sheetData sheetId="759"/>
+      <sheetData sheetId="760"/>
+      <sheetData sheetId="761"/>
+      <sheetData sheetId="762"/>
+      <sheetData sheetId="763"/>
+      <sheetData sheetId="764"/>
+      <sheetData sheetId="765"/>
+      <sheetData sheetId="766"/>
+      <sheetData sheetId="767"/>
+      <sheetData sheetId="768"/>
+      <sheetData sheetId="769"/>
+      <sheetData sheetId="770"/>
+      <sheetData sheetId="771"/>
+      <sheetData sheetId="772"/>
+      <sheetData sheetId="773"/>
+      <sheetData sheetId="774"/>
+      <sheetData sheetId="775"/>
+      <sheetData sheetId="776"/>
+      <sheetData sheetId="777"/>
+      <sheetData sheetId="778" refreshError="1"/>
+      <sheetData sheetId="779" refreshError="1"/>
+      <sheetData sheetId="780" refreshError="1"/>
+      <sheetData sheetId="781" refreshError="1"/>
+      <sheetData sheetId="782" refreshError="1"/>
+      <sheetData sheetId="783" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6452,7 +6729,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6487,7 +6764,7 @@
 </externalLink>
 </file>
 
-<file path=xl/externalLinks/externalLink6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -6500,6 +6777,7 @@
       <sheetName val="ALOBS"/>
       <sheetName val="Edu-5"/>
       <sheetName val="LYDS4 (2)"/>
+      <sheetName val="Database"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -6511,285 +6789,7 @@
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink7.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="summary"/>
-      <sheetName val="Graceano Lopez"/>
-      <sheetName val="Ernesto Rondon HS"/>
-      <sheetName val="Juan Luna ES"/>
-      <sheetName val="Pamplona ES"/>
-      <sheetName val="Ilaya ES"/>
-      <sheetName val="Ernesto Rondon HS (2)"/>
-      <sheetName val="RESPSCI"/>
-      <sheetName val="Paranaque NHS"/>
-      <sheetName val="Talon ES"/>
-      <sheetName val="Zapote ES"/>
-      <sheetName val="Quantity Take-off"/>
-      <sheetName val="Graceano Lopez Jaena ES"/>
-      <sheetName val="A. Albert ES"/>
-      <sheetName val="Las Pinas HS (CAA)"/>
-      <sheetName val="Database"/>
-      <sheetName val="Graceano_Lopez2"/>
-      <sheetName val="Ernesto_Rondon_HS2"/>
-      <sheetName val="Juan_Luna_ES2"/>
-      <sheetName val="Pamplona_ES2"/>
-      <sheetName val="Ilaya_ES2"/>
-      <sheetName val="Ernesto_Rondon_HS_(2)2"/>
-      <sheetName val="Paranaque_NHS2"/>
-      <sheetName val="Talon_ES2"/>
-      <sheetName val="Zapote_ES2"/>
-      <sheetName val="Quantity_Take-off2"/>
-      <sheetName val="Graceano_Lopez_Jaena_ES2"/>
-      <sheetName val="A__Albert_ES2"/>
-      <sheetName val="Las_Pinas_HS_(CAA)2"/>
-      <sheetName val="Graceano_Lopez"/>
-      <sheetName val="Ernesto_Rondon_HS"/>
-      <sheetName val="Juan_Luna_ES"/>
-      <sheetName val="Pamplona_ES"/>
-      <sheetName val="Ilaya_ES"/>
-      <sheetName val="Ernesto_Rondon_HS_(2)"/>
-      <sheetName val="Paranaque_NHS"/>
-      <sheetName val="Talon_ES"/>
-      <sheetName val="Zapote_ES"/>
-      <sheetName val="Quantity_Take-off"/>
-      <sheetName val="Graceano_Lopez_Jaena_ES"/>
-      <sheetName val="A__Albert_ES"/>
-      <sheetName val="Las_Pinas_HS_(CAA)"/>
-      <sheetName val="Graceano_Lopez1"/>
-      <sheetName val="Ernesto_Rondon_HS1"/>
-      <sheetName val="Juan_Luna_ES1"/>
-      <sheetName val="Pamplona_ES1"/>
-      <sheetName val="Ilaya_ES1"/>
-      <sheetName val="Ernesto_Rondon_HS_(2)1"/>
-      <sheetName val="Paranaque_NHS1"/>
-      <sheetName val="Talon_ES1"/>
-      <sheetName val="Zapote_ES1"/>
-      <sheetName val="Quantity_Take-off1"/>
-      <sheetName val="Graceano_Lopez_Jaena_ES1"/>
-      <sheetName val="A__Albert_ES1"/>
-      <sheetName val="Las_Pinas_HS_(CAA)1"/>
-      <sheetName val="Contractor"/>
-      <sheetName val="DECS 2cl OMS (2)"/>
-      <sheetName val="buhelebongES"/>
-      <sheetName val="Max"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
-      <sheetData sheetId="32" refreshError="1"/>
-      <sheetData sheetId="33" refreshError="1"/>
-      <sheetData sheetId="34" refreshError="1"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43" refreshError="1"/>
-      <sheetData sheetId="44" refreshError="1"/>
-      <sheetData sheetId="45" refreshError="1"/>
-      <sheetData sheetId="46" refreshError="1"/>
-      <sheetData sheetId="47" refreshError="1"/>
-      <sheetData sheetId="48" refreshError="1"/>
-      <sheetData sheetId="49" refreshError="1"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink8.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="POW"/>
-      <sheetName val="Lupang Pangako"/>
-      <sheetName val="Database"/>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-      <sheetName val="Sheet3"/>
-      <sheetName val="SUMMARY"/>
-      <sheetName val="Lupang_Pangako"/>
-      <sheetName val="Max"/>
-      <sheetName val="Lupang_Pangako6"/>
-      <sheetName val="Lupang_Pangako1"/>
-      <sheetName val="Lupang_Pangako4"/>
-      <sheetName val="Lupang_Pangako2"/>
-      <sheetName val="Lupang_Pangako3"/>
-      <sheetName val="Lupang_Pangako5"/>
-      <sheetName val="Lupang_Pangako7"/>
-      <sheetName val="Lupang_Pangako8"/>
-      <sheetName val="Lupang_Pangako10"/>
-      <sheetName val="Lupang_Pangako9"/>
-      <sheetName val="Target for 2019"/>
-      <sheetName val="Per Program"/>
-      <sheetName val="REPAIR 2017"/>
-      <sheetName val="Repair 2018"/>
-      <sheetName val="REPAIR 2019"/>
-      <sheetName val="Electrification 2018"/>
-      <sheetName val="buhelebongES"/>
-      <sheetName val="EDU4"/>
-      <sheetName val="dbase"/>
-      <sheetName val="Lupang_Pangako11"/>
-      <sheetName val="Target_for_2019"/>
-      <sheetName val="Per_Program"/>
-      <sheetName val="REPAIR_2017"/>
-      <sheetName val="Repair_2018"/>
-      <sheetName val="REPAIR_2019"/>
-      <sheetName val="Electrification_2018"/>
-      <sheetName val="SOM"/>
-      <sheetName val="DO 71 s 2013"/>
-      <sheetName val="LIBRARY"/>
-      <sheetName val="101(2)e"/>
-      <sheetName val="101(2)g"/>
-      <sheetName val="101(2)c"/>
-      <sheetName val="101(2)f"/>
-      <sheetName val="Worksheet"/>
-      <sheetName val="Lupang_Pangako12"/>
-      <sheetName val="Target_for_20191"/>
-      <sheetName val="Per_Program1"/>
-      <sheetName val="REPAIR_20171"/>
-      <sheetName val="Repair_20181"/>
-      <sheetName val="REPAIR_20191"/>
-      <sheetName val="Electrification_20181"/>
-      <sheetName val="rates"/>
-      <sheetName val="RATE"/>
-      <sheetName val="ABC"/>
-      <sheetName val="general"/>
-      <sheetName val="ACCOMP. REPORT sub"/>
-      <sheetName val="TABLES"/>
-      <sheetName val="DRSB_Weight"/>
-      <sheetName val="EQUIPMENT"/>
-      <sheetName val="nm"/>
-      <sheetName val="Payitems"/>
-      <sheetName val="Basis (2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35" refreshError="1"/>
-      <sheetData sheetId="36" refreshError="1"/>
-      <sheetData sheetId="37" refreshError="1"/>
-      <sheetData sheetId="38" refreshError="1"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41" refreshError="1"/>
-      <sheetData sheetId="42" refreshError="1"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50" refreshError="1"/>
-      <sheetData sheetId="51" refreshError="1"/>
-      <sheetData sheetId="52" refreshError="1"/>
-      <sheetData sheetId="53" refreshError="1"/>
-      <sheetData sheetId="54" refreshError="1"/>
-      <sheetData sheetId="55" refreshError="1"/>
-      <sheetData sheetId="56" refreshError="1"/>
-      <sheetData sheetId="57" refreshError="1"/>
-      <sheetData sheetId="58" refreshError="1"/>
-      <sheetData sheetId="59" refreshError="1"/>
-      <sheetData sheetId="60" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink9.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Enrolees&amp;Graduated"/>
-      <sheetName val="Classrooms"/>
-      <sheetName val="Drop-out"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7098,10 +7098,10 @@
   <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D18" sqref="D18:D19"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
-      <selection pane="bottomRight" activeCell="X1" sqref="X1"/>
+      <selection pane="bottomRight" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
added index for all files
</commit_message>
<xml_diff>
--- a/FINAL-PROGRAMS/FINAL- ALS-CLC 2024 as of May 2025.xlsx
+++ b/FINAL-PROGRAMS/FINAL- ALS-CLC 2024 as of May 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Work - Lawrence\Documents\DepEd_scripts\FINAL-PROGRAMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C121289C-F2E4-4F5D-820B-18041376E19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D2E7F0-032D-4DB0-BB54-5030B46AADC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -56,7 +56,6 @@
     <definedName name="_EDU2">[2]EDU4!$G$10</definedName>
     <definedName name="_Fill" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Fill" hidden="1">#REF!</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ALS-CLC 2024'!$A$1:$W$5</definedName>
     <definedName name="_Key1" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="_Key1" hidden="1">#REF!</definedName>
     <definedName name="_Key2" localSheetId="0" hidden="1">#REF!</definedName>
@@ -270,12 +269,12 @@
     <definedName name="ppmp2">#REF!</definedName>
     <definedName name="Prin" localSheetId="0">#REF!</definedName>
     <definedName name="Prin">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$A$1:$I$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'ALS-CLC 2024'!$B$2:$J$5</definedName>
     <definedName name="PRINT_AREA_MI" localSheetId="0">#REF!</definedName>
     <definedName name="PRINT_AREA_MI">#REF!</definedName>
     <definedName name="print_area_Mil" localSheetId="0">#REF!</definedName>
     <definedName name="print_area_Mil">#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!$1:$1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'ALS-CLC 2024'!#REF!</definedName>
     <definedName name="Print_Titles_MI" localSheetId="0">'[15]Enrolees&amp;Graduated'!$A$1:$IV$6,'[15]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
     <definedName name="Print_Titles_MI">'[16]Enrolees&amp;Graduated'!$A$1:$IV$6,'[16]Enrolees&amp;Graduated'!$A$1:$A$65536</definedName>
     <definedName name="procured" localSheetId="0" hidden="1">#REF!</definedName>
@@ -411,34 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
-  <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Division</t>
-  </si>
-  <si>
-    <t>School ID</t>
-  </si>
-  <si>
-    <t>School Name</t>
-  </si>
-  <si>
-    <t>Municipality</t>
-  </si>
-  <si>
-    <t>Leg District</t>
-  </si>
-  <si>
-    <t>No. of Sites</t>
-  </si>
-  <si>
-    <t>Scope of Work</t>
-  </si>
-  <si>
-    <t>Total Allocation</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="87">
   <si>
     <t>CONTRACT AMOUNT</t>
   </si>
@@ -447,39 +419,6 @@
   </si>
   <si>
     <t>PERCENTAGE OF COMPLETION</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Target Completion Date </t>
-  </si>
-  <si>
-    <t>Actual Date of Completion</t>
-  </si>
-  <si>
-    <t>Project ID</t>
-  </si>
-  <si>
-    <t>Contract ID</t>
-  </si>
-  <si>
-    <t>Issuance of Invitation to Bid</t>
-  </si>
-  <si>
-    <t>Pre-Submission Conference</t>
-  </si>
-  <si>
-    <t>Bid Opening</t>
-  </si>
-  <si>
-    <t>Issuance of Resolution to Award</t>
-  </si>
-  <si>
-    <t>Issuance of Notice to Proceed</t>
-  </si>
-  <si>
-    <t>Name of Contractor</t>
-  </si>
-  <si>
-    <t>Other Remarks</t>
   </si>
   <si>
     <t>CARAGA</t>
@@ -671,6 +610,69 @@
   </si>
   <si>
     <t>actual target completion was adjusted due to contractor request for extension regarding weather condition</t>
+  </si>
+  <si>
+    <t>REGION</t>
+  </si>
+  <si>
+    <t>DIVISION</t>
+  </si>
+  <si>
+    <t>SCHOOL ID</t>
+  </si>
+  <si>
+    <t>SCHOOL NAME</t>
+  </si>
+  <si>
+    <t>MUNICIPALITY</t>
+  </si>
+  <si>
+    <t>LEG DISTRICT</t>
+  </si>
+  <si>
+    <t>NO. OF SITES</t>
+  </si>
+  <si>
+    <t>SCOPE OF WORK</t>
+  </si>
+  <si>
+    <t>TOTAL ALLOCATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TARGET COMPLETION DATE </t>
+  </si>
+  <si>
+    <t>ACTUAL DATE OF COMPLETION</t>
+  </si>
+  <si>
+    <t>PROJECT ID</t>
+  </si>
+  <si>
+    <t>CONTRACT ID</t>
+  </si>
+  <si>
+    <t>ISSUANCE OF INVITATION TO BID</t>
+  </si>
+  <si>
+    <t>PRE-SUBMISSION CONFERENCE</t>
+  </si>
+  <si>
+    <t>BID OPENING</t>
+  </si>
+  <si>
+    <t>ISSUANCE OF RESOLUTION TO AWARD</t>
+  </si>
+  <si>
+    <t>ISSUANCE OF NOTICE TO PROCEED</t>
+  </si>
+  <si>
+    <t>NAME OF CONTRACTOR</t>
+  </si>
+  <si>
+    <t>OTHER REMARKS</t>
+  </si>
+  <si>
+    <t>INDEX (DO NOT MODIFY)</t>
   </si>
 </sst>
 </file>
@@ -7095,400 +7097,415 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:W5"/>
+  <dimension ref="A1:X5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D18" sqref="D18:D19"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18:D19"/>
-      <selection pane="bottomRight" sqref="A1:A1048576"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.26953125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="32.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.453125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="29.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="36" style="15" customWidth="1"/>
-    <col min="10" max="10" width="16.81640625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.81640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.81640625" style="4" customWidth="1"/>
-    <col min="13" max="14" width="16.81640625" style="5" customWidth="1"/>
-    <col min="15" max="16" width="16.81640625" style="1" customWidth="1"/>
-    <col min="17" max="20" width="16.81640625" style="5" customWidth="1"/>
-    <col min="21" max="21" width="29.54296875" style="5" customWidth="1"/>
-    <col min="22" max="23" width="16.81640625" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="9.1796875" style="1"/>
+    <col min="2" max="2" width="19.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="29" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="35.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.453125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7265625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="29.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="36" style="15" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="16.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.81640625" style="4" customWidth="1"/>
+    <col min="14" max="15" width="16.81640625" style="5" customWidth="1"/>
+    <col min="16" max="17" width="16.81640625" style="1" customWidth="1"/>
+    <col min="18" max="21" width="16.81640625" style="5" customWidth="1"/>
+    <col min="22" max="22" width="29.54296875" style="5" customWidth="1"/>
+    <col min="23" max="24" width="16.81640625" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="13" customFormat="1" ht="60.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" s="13" customFormat="1" ht="60.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="L1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="M1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="N1" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="P1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="R1" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="14">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="C2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="D2" s="16">
+        <v>131508</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="F2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="G2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="H2" s="17">
+        <v>1</v>
+      </c>
+      <c r="I2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J2" s="18">
+        <v>14141414.140000001</v>
+      </c>
+      <c r="K2" s="19">
+        <v>14070707.07</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="10" t="s">
+      <c r="M2" s="20">
+        <v>1</v>
+      </c>
+      <c r="N2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="O2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="P2" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="Q2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="10" t="s">
+      <c r="S2" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="T2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="U2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="12" t="s">
+      <c r="V2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="W2" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="X2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="12" t="s">
+    </row>
+    <row r="3" spans="1:24" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="10" t="s">
+      <c r="C3" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="D3" s="16">
+        <v>100684</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>22</v>
       </c>
+      <c r="F3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="17">
+        <v>1</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="18">
+        <v>12871493.449999999</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="20">
+        <v>0.8</v>
+      </c>
+      <c r="N3" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="21"/>
+      <c r="P3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="W3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="X3" s="16" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="16" t="s">
+    <row r="4" spans="1:24" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="16">
+        <v>300690</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="17">
+        <v>1</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="18">
+        <v>12446387.1</v>
+      </c>
+      <c r="K4" s="19">
+        <v>10458975.449999999</v>
+      </c>
+      <c r="L4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="M4" s="20">
+        <v>0.7</v>
+      </c>
+      <c r="N4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="21"/>
+      <c r="P4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="R4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="S4" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="U4" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="16" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="14">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="16">
+        <v>301596</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="17">
+        <v>1</v>
+      </c>
+      <c r="I5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="16">
-        <v>131508</v>
-      </c>
-      <c r="D2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="17">
+      <c r="J5" s="18">
+        <v>16540705.310000001</v>
+      </c>
+      <c r="K5" s="19">
+        <v>16458637.91</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M5" s="20">
         <v>1</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="I2" s="18">
-        <v>14141414.140000001</v>
-      </c>
-      <c r="J2" s="19">
-        <v>14070707.07</v>
-      </c>
-      <c r="K2" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L2" s="20">
-        <v>1</v>
-      </c>
-      <c r="M2" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="V2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="16">
-        <v>100684</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="17">
-        <v>1</v>
-      </c>
-      <c r="H3" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I3" s="18">
-        <v>12871493.449999999</v>
-      </c>
-      <c r="J3" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L3" s="20">
-        <v>0.8</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="21"/>
-      <c r="O3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="21" t="s">
-        <v>52</v>
-      </c>
-      <c r="T3" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="16" t="s">
+      <c r="N5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="O5" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="16">
-        <v>300690</v>
-      </c>
-      <c r="D4" s="16" t="s">
+      <c r="P5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="Q5" s="16"/>
+      <c r="R5" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="S5" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="17">
-        <v>1</v>
-      </c>
-      <c r="H4" s="16" t="s">
+      <c r="T5" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="I4" s="18">
-        <v>12446387.1</v>
-      </c>
-      <c r="J4" s="19">
-        <v>10458975.449999999</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="L4" s="20">
-        <v>0.7</v>
-      </c>
-      <c r="M4" s="21" t="s">
+      <c r="U5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="V5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="N4" s="21"/>
-      <c r="O4" s="16" t="s">
+      <c r="W5" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="X5" s="16" t="s">
         <v>65</v>
-      </c>
-      <c r="Q4" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="R4" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="S4" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="T4" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="U4" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="V4" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="W4" s="16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" s="14" customFormat="1" ht="154.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="16">
-        <v>301596</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="17">
-        <v>1</v>
-      </c>
-      <c r="H5" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" s="18">
-        <v>16540705.310000001</v>
-      </c>
-      <c r="J5" s="19">
-        <v>16458637.91</v>
-      </c>
-      <c r="K5" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="20">
-        <v>1</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="O5" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="R5" s="21" t="s">
-        <v>81</v>
-      </c>
-      <c r="S5" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="T5" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="V5" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="W5" s="16" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W5" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="C1:C2 C4 C6:C1048576">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+  <conditionalFormatting sqref="D3">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C3">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  <conditionalFormatting sqref="D4 D6:D1048576 D1:D2">
+    <cfRule type="duplicateValues" dxfId="2" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
+  <conditionalFormatting sqref="D5">
     <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:W5">
+  <conditionalFormatting sqref="K2:X5">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(J2))=0</formula>
+      <formula>LEN(TRIM(K2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>

</xml_diff>